<commit_message>
Show the skiped item based on the TODAY date
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/08-various-bounds/08-various-bounds.xlsx
+++ b/ampl-data-input-excel/08-various-bounds/08-various-bounds.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="experts" sheetId="1" state="visible" r:id="rId3"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="89">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -105,6 +105,18 @@
     <t xml:space="preserve">3 tasks, 1 ubday(1), 2 ubsum</t>
   </si>
   <si>
+    <t xml:space="preserve">DEV.Żaklina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">without any task</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PM.Remigiusz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">many tasks in the past</t>
+  </si>
+  <si>
     <t xml:space="preserve">Start day</t>
   </si>
   <si>
@@ -177,6 +189,18 @@
     <t xml:space="preserve">DEV.p21.m</t>
   </si>
   <si>
+    <t xml:space="preserve">PM.old.a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PM.old.b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PM.old.c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SA.free.1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Expert</t>
   </si>
   <si>
@@ -187,6 +211,12 @@
   </si>
   <si>
     <t xml:space="preserve">Upper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24.Nov</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24.Dec</t>
   </si>
   <si>
     <t xml:space="preserve">25.Jan</t>
@@ -369,16 +399,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -415,6 +441,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -422,12 +452,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -448,6 +478,18 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -637,23 +679,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="36.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="36.04"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -661,7 +703,7 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -669,7 +711,7 @@
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -677,7 +719,7 @@
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -685,7 +727,7 @@
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -693,7 +735,7 @@
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -701,7 +743,7 @@
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -709,7 +751,7 @@
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
     </row>
@@ -717,7 +759,7 @@
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -725,7 +767,7 @@
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -733,7 +775,7 @@
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -741,12 +783,25 @@
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2"/>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -764,39 +819,39 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.86"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="4" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="3" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>51</v>
+      <c r="A1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="C2" s="19" t="n">
         <v>100</v>
@@ -806,11 +861,11 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="C3" s="19" t="n">
         <v>100</v>
@@ -820,11 +875,11 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="C4" s="19" t="n">
         <v>100</v>
@@ -834,11 +889,11 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="C5" s="19" t="n">
         <v>0</v>
@@ -848,11 +903,11 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="C6" s="19" t="n">
         <v>0</v>
@@ -862,22 +917,102 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="A7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>200</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="A8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>201</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="A9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>206</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -895,7 +1030,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -903,16 +1038,21 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
-        <v>68</v>
+      <c r="A1" s="6" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="n">
+        <v>45413</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="10" t="n">
         <v>45651</v>
       </c>
     </row>
@@ -934,66 +1074,66 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="19.48"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="19.48"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>76</v>
+      <c r="A1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="B2" s="4" t="n">
+      <c r="A2" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="22" t="n">
         <v>100</v>
       </c>
-      <c r="D2" s="20" t="n">
+      <c r="D2" s="23" t="n">
         <v>45642</v>
       </c>
-      <c r="E2" s="20" t="n">
+      <c r="E2" s="23" t="n">
         <v>45778</v>
       </c>
-      <c r="F2" s="20" t="n">
+      <c r="F2" s="23" t="n">
         <v>45642</v>
       </c>
-      <c r="G2" s="20" t="n">
+      <c r="G2" s="23" t="n">
         <v>45778</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>78</v>
+      <c r="H2" s="22" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1012,324 +1152,380 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="4" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="3" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>26</v>
+      <c r="B1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="9" t="n">
+      <c r="A2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="8" t="n">
         <v>45642</v>
       </c>
-      <c r="C2" s="9" t="n">
+      <c r="C2" s="8" t="n">
         <v>45749</v>
       </c>
-      <c r="D2" s="10" t="n">
+      <c r="D2" s="9" t="n">
         <v>400</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="9" t="n">
+      <c r="A3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="8" t="n">
         <v>45642</v>
       </c>
-      <c r="C3" s="9" t="n">
+      <c r="C3" s="8" t="n">
         <v>45749</v>
       </c>
-      <c r="D3" s="10" t="n">
+      <c r="D3" s="9" t="n">
         <v>420</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="9" t="n">
+      <c r="A4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="8" t="n">
         <v>45642</v>
       </c>
-      <c r="C4" s="9" t="n">
+      <c r="C4" s="8" t="n">
         <v>45749</v>
       </c>
-      <c r="D4" s="10" t="n">
+      <c r="D4" s="9" t="n">
         <v>430</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="9" t="n">
+      <c r="A5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="8" t="n">
         <v>45642</v>
       </c>
-      <c r="C5" s="9" t="n">
+      <c r="C5" s="8" t="n">
         <v>45749</v>
       </c>
-      <c r="D5" s="10" t="n">
+      <c r="D5" s="9" t="n">
         <v>440</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="9" t="n">
+      <c r="A6" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="8" t="n">
         <v>45642</v>
       </c>
-      <c r="C6" s="9" t="n">
+      <c r="C6" s="8" t="n">
         <v>45718</v>
       </c>
-      <c r="D6" s="10" t="n">
+      <c r="D6" s="9" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="9" t="n">
+      <c r="A7" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="8" t="n">
         <v>45642</v>
       </c>
-      <c r="C7" s="9" t="n">
+      <c r="C7" s="8" t="n">
         <v>45749</v>
       </c>
-      <c r="D7" s="10" t="n">
+      <c r="D7" s="9" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="9" t="n">
+      <c r="A8" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="8" t="n">
         <v>45642</v>
       </c>
-      <c r="C8" s="9" t="n">
+      <c r="C8" s="8" t="n">
         <v>45718</v>
       </c>
-      <c r="D8" s="10" t="n">
+      <c r="D8" s="9" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="9" t="n">
+      <c r="A9" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="8" t="n">
         <v>45642</v>
       </c>
-      <c r="C9" s="9" t="n">
+      <c r="C9" s="8" t="n">
         <v>45749</v>
       </c>
-      <c r="D9" s="10" t="n">
+      <c r="D9" s="9" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="9" t="n">
+      <c r="A10" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="8" t="n">
         <v>45642</v>
       </c>
-      <c r="C10" s="9" t="n">
+      <c r="C10" s="8" t="n">
         <v>45718</v>
       </c>
-      <c r="D10" s="10" t="n">
+      <c r="D10" s="9" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="9" t="n">
+      <c r="A11" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="8" t="n">
         <v>45642</v>
       </c>
-      <c r="C11" s="9" t="n">
+      <c r="C11" s="8" t="n">
         <v>45749</v>
       </c>
-      <c r="D11" s="10" t="n">
+      <c r="D11" s="9" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="9" t="n">
+      <c r="A12" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="8" t="n">
         <v>45642</v>
       </c>
-      <c r="C12" s="9" t="n">
+      <c r="C12" s="8" t="n">
         <v>45718</v>
       </c>
-      <c r="D12" s="10" t="n">
+      <c r="D12" s="9" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="9" t="n">
+      <c r="A13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="8" t="n">
         <v>45642</v>
       </c>
-      <c r="C13" s="9" t="n">
+      <c r="C13" s="8" t="n">
         <v>45749</v>
       </c>
-      <c r="D13" s="10" t="n">
+      <c r="D13" s="9" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="9" t="n">
+      <c r="A14" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="8" t="n">
         <v>45642</v>
       </c>
-      <c r="C14" s="9" t="n">
+      <c r="C14" s="8" t="n">
         <v>45718</v>
       </c>
-      <c r="D14" s="10" t="n">
+      <c r="D14" s="9" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="9" t="n">
+      <c r="A15" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="8" t="n">
         <v>45642</v>
       </c>
-      <c r="C15" s="9" t="n">
+      <c r="C15" s="8" t="n">
         <v>45749</v>
       </c>
-      <c r="D15" s="10" t="n">
+      <c r="D15" s="9" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="9" t="n">
+      <c r="A16" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="8" t="n">
         <v>45642</v>
       </c>
-      <c r="C16" s="9" t="n">
+      <c r="C16" s="8" t="n">
         <v>45779</v>
       </c>
-      <c r="D16" s="10" t="n">
+      <c r="D16" s="9" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="9" t="n">
+      <c r="A17" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="8" t="n">
         <v>45642</v>
       </c>
-      <c r="C17" s="9" t="n">
+      <c r="C17" s="8" t="n">
         <v>45718</v>
       </c>
-      <c r="D17" s="10" t="n">
+      <c r="D17" s="9" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="9" t="n">
+      <c r="A18" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="8" t="n">
         <v>45642</v>
       </c>
-      <c r="C18" s="9" t="n">
+      <c r="C18" s="8" t="n">
         <v>45749</v>
       </c>
-      <c r="D18" s="10" t="n">
+      <c r="D18" s="9" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" s="9" t="n">
+      <c r="A19" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="8" t="n">
         <v>45642</v>
       </c>
-      <c r="C19" s="9" t="n">
+      <c r="C19" s="8" t="n">
         <v>45779</v>
       </c>
-      <c r="D19" s="10" t="n">
+      <c r="D19" s="9" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B20" s="9" t="n">
+      <c r="A20" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="8" t="n">
         <v>45642</v>
       </c>
-      <c r="C20" s="9" t="n">
+      <c r="C20" s="8" t="n">
         <v>45718</v>
       </c>
-      <c r="D20" s="10" t="n">
+      <c r="D20" s="9" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B21" s="9" t="n">
+      <c r="A21" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="8" t="n">
         <v>45642</v>
       </c>
-      <c r="C21" s="9" t="n">
+      <c r="C21" s="8" t="n">
         <v>45749</v>
       </c>
-      <c r="D21" s="10" t="n">
+      <c r="D21" s="9" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B22" s="9" t="n">
+      <c r="A22" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="8" t="n">
         <v>45642</v>
       </c>
-      <c r="C22" s="9" t="n">
+      <c r="C22" s="8" t="n">
         <v>45779</v>
       </c>
-      <c r="D22" s="10" t="n">
+      <c r="D22" s="9" t="n">
         <v>200</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="10" t="n">
+        <v>45292</v>
+      </c>
+      <c r="C23" s="10" t="n">
+        <v>45324</v>
+      </c>
+      <c r="D23" s="3" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="10" t="n">
+        <v>45352</v>
+      </c>
+      <c r="C24" s="10" t="n">
+        <v>45384</v>
+      </c>
+      <c r="D24" s="3" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="10" t="n">
+        <v>45383</v>
+      </c>
+      <c r="C25" s="10" t="n">
+        <v>45414</v>
+      </c>
+      <c r="D25" s="3" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="10" t="n">
+        <v>45658</v>
+      </c>
+      <c r="C26" s="10" t="n">
+        <v>45751</v>
+      </c>
+      <c r="D26" s="3" t="n">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1348,10 +1544,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1361,11 +1557,11 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>49</v>
+      <c r="A1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1373,7 +1569,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1381,7 +1577,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1389,7 +1585,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1397,7 +1593,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1405,7 +1601,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1413,7 +1609,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1421,7 +1617,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1429,7 +1625,7 @@
         <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1437,7 +1633,7 @@
         <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1445,7 +1641,7 @@
         <v>14</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1453,7 +1649,7 @@
         <v>16</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1461,7 +1657,7 @@
         <v>16</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1469,7 +1665,7 @@
         <v>18</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1477,7 +1673,7 @@
         <v>18</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1485,7 +1681,7 @@
         <v>18</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1493,7 +1689,7 @@
         <v>20</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1501,7 +1697,7 @@
         <v>20</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1509,7 +1705,7 @@
         <v>20</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1517,7 +1713,7 @@
         <v>22</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1525,7 +1721,7 @@
         <v>22</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1533,7 +1729,31 @@
         <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1555,34 +1775,34 @@
   <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K22" activeCellId="0" sqref="K22"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.76"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="3" style="4" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="3" style="3" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>51</v>
+      <c r="A1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1590,7 +1810,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C2" s="11" t="n">
         <v>45642</v>
@@ -1606,11 +1826,11 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>29</v>
+      <c r="B3" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="C3" s="12" t="n">
         <v>45642</v>
@@ -1618,19 +1838,19 @@
       <c r="D3" s="12" t="n">
         <v>45646</v>
       </c>
-      <c r="E3" s="8" t="n">
+      <c r="E3" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="F3" s="8" t="n">
+      <c r="F3" s="7" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>29</v>
+      <c r="B4" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="C4" s="12" t="n">
         <v>45649</v>
@@ -1638,30 +1858,72 @@
       <c r="D4" s="12" t="n">
         <v>45653</v>
       </c>
-      <c r="E4" s="8" t="n">
+      <c r="E4" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="F4" s="8" t="n">
+      <c r="F4" s="7" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="10" t="n">
+        <v>45292</v>
+      </c>
+      <c r="D5" s="10" t="n">
+        <v>45324</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="10" t="n">
+        <v>45352</v>
+      </c>
+      <c r="D6" s="10" t="n">
+        <v>45384</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="10" t="n">
+        <v>45383</v>
+      </c>
+      <c r="D7" s="10" t="n">
+        <v>45414</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="1"/>
@@ -2060,35 +2322,35 @@
   <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.76"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="4" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="3" width="11.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>51</v>
+      <c r="A1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2096,7 +2358,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C2" s="11" t="n">
         <v>45642</v>
@@ -2112,19 +2374,64 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="10" t="n">
+        <v>45292</v>
+      </c>
+      <c r="D3" s="10" t="n">
+        <v>45296</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="10" t="n">
+        <v>45352</v>
+      </c>
+      <c r="D4" s="10" t="n">
+        <v>45361</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="10" t="n">
+        <v>45383</v>
+      </c>
+      <c r="D5" s="10" t="n">
+        <v>45389</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="1"/>
@@ -2470,30 +2777,30 @@
   <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.76"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="2" style="4" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="2" style="3" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>51</v>
+      <c r="A1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2565,22 +2872,55 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="10" t="n">
+        <v>45292</v>
+      </c>
+      <c r="C6" s="10" t="n">
+        <v>45324</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="10" t="n">
+        <v>45352</v>
+      </c>
+      <c r="C7" s="10" t="n">
+        <v>45384</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="10" t="n">
+        <v>45383</v>
+      </c>
+      <c r="C8" s="10" t="n">
+        <v>45414</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1"/>
@@ -2973,35 +3313,35 @@
   <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.76"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="4" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="3" width="11.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>51</v>
+      <c r="A1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3009,7 +3349,7 @@
         <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C2" s="11" t="n">
         <v>45642</v>
@@ -3029,7 +3369,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C3" s="11" t="n">
         <v>45642</v>
@@ -3049,7 +3389,7 @@
         <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C4" s="11" t="n">
         <v>45642</v>
@@ -3069,7 +3409,7 @@
         <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C5" s="11" t="n">
         <v>45642</v>
@@ -3089,7 +3429,7 @@
         <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C6" s="11" t="n">
         <v>45642</v>
@@ -3105,9 +3445,24 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="10" t="n">
+        <v>45292</v>
+      </c>
+      <c r="D7" s="10" t="n">
+        <v>45324</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="1"/>
@@ -3443,183 +3798,196 @@
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="2" style="4" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="2" style="3" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>51</v>
+      <c r="A1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
+      <c r="A2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="10" t="n">
+        <v>45292</v>
+      </c>
+      <c r="C2" s="10" t="n">
+        <v>45301</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3640,95 +4008,106 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="4" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="3" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>25</v>
+      <c r="B1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>54</v>
+      <c r="A2" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="14" t="n">
+        <v>45597</v>
+      </c>
+      <c r="C2" s="14" t="n">
+        <v>45626</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>57</v>
+      <c r="A3" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="14" t="n">
+        <v>45627</v>
+      </c>
+      <c r="C3" s="14" t="n">
+        <v>45636</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="15" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="15" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="A7" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+      <c r="A8" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Delete code removing items before TODAY. Adjust examples
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/08-various-bounds/08-various-bounds.xlsx
+++ b/ampl-data-input-excel/08-various-bounds/08-various-bounds.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="experts" sheetId="1" state="visible" r:id="rId3"/>
@@ -30,8 +30,417 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author>Unknown Author</author>
+  </authors>
+  <commentList>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Has Expert any task?</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author>Unknown Author</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Valid expert?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Valid period?</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author>Unknown Author</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Are dates OK?</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author>Unknown Author</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Is task assign to an Expert?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Should task be included?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Are date OK?</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author>Unknown Author</author>
+  </authors>
+  <commentList>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Valid expert?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Valid task?</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author>Unknown Author</author>
+  </authors>
+  <commentList>
+    <comment ref="G1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Valid expert?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Valid task?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Are date OK?</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author>Unknown Author</author>
+  </authors>
+  <commentList>
+    <comment ref="G1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Valid expert?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Valid task?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Are date OK?</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author>Unknown Author</author>
+  </authors>
+  <commentList>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Valid expert?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Are date OK?</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author>Unknown Author</author>
+  </authors>
+  <commentList>
+    <comment ref="G1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Valid expert?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Valid task?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Are date OK?</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author>Unknown Author</author>
+  </authors>
+  <commentList>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Valid expert?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Are date OK?</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author>Unknown Author</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Are date OK?</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="75">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -105,18 +514,6 @@
     <t xml:space="preserve">3 tasks, 1 ubday(1), 2 ubsum</t>
   </si>
   <si>
-    <t xml:space="preserve">DEV.Żaklina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">without any task</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PM.Remigiusz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">many tasks in the past</t>
-  </si>
-  <si>
     <t xml:space="preserve">Start day</t>
   </si>
   <si>
@@ -189,18 +586,6 @@
     <t xml:space="preserve">DEV.p21.m</t>
   </si>
   <si>
-    <t xml:space="preserve">PM.old.a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PM.old.b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PM.old.c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SA.free.1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Expert</t>
   </si>
   <si>
@@ -222,48 +607,18 @@
     <t xml:space="preserve">25.Jan</t>
   </si>
   <si>
-    <t xml:space="preserve">2024-12-11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-01-15</t>
-  </si>
-  <si>
     <t xml:space="preserve">25.Feb</t>
   </si>
   <si>
-    <t xml:space="preserve">2025-01-16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-02-13</t>
-  </si>
-  <si>
     <t xml:space="preserve">25.Mar</t>
   </si>
   <si>
-    <t xml:space="preserve">2025-02-14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-03-16</t>
-  </si>
-  <si>
     <t xml:space="preserve">25.Apr</t>
   </si>
   <si>
-    <t xml:space="preserve">2025-03-17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-04-14</t>
-  </si>
-  <si>
     <t xml:space="preserve">25.May</t>
   </si>
   <si>
-    <t xml:space="preserve">2025-04-15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-05-18</t>
-  </si>
-  <si>
     <t xml:space="preserve">Period</t>
   </si>
   <si>
@@ -294,7 +649,19 @@
     <t xml:space="preserve">Solver</t>
   </si>
   <si>
-    <t xml:space="preserve">2024-12-15</t>
+    <t xml:space="preserve">Last day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is T:start OK?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is T:end OK?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is H:start OK?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is H:end OK?</t>
   </si>
   <si>
     <t xml:space="preserve">highs</t>
@@ -304,12 +671,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -344,13 +712,27 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD8CE"/>
+        <bgColor rgb="FFFFD7D7"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -360,8 +742,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF993300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFD7"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD7D7"/>
+        <bgColor rgb="FFFFD8CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -399,7 +793,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -408,39 +802,55 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -448,23 +858,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -472,15 +882,11 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -488,11 +894,23 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -530,7 +948,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFFFD7D7"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -546,7 +964,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFD8CE"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -679,23 +1097,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="36.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.19"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="b">
+        <f aca="false">AND(C2:C985)</f>
         <v>1</v>
       </c>
     </row>
@@ -706,6 +1129,10 @@
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C2" s="5" t="b">
+        <f aca="false">COUNTIF(links!$A$1:$A$868, A2) &gt; 0</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -714,6 +1141,10 @@
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C3" s="5" t="n">
+        <f aca="false">COUNTIF(links!$A$1:$A$868, A3) &gt; 0</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -722,6 +1153,10 @@
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="C4" s="5" t="n">
+        <f aca="false">COUNTIF(links!$A$1:$A$868, A4) &gt; 0</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -730,6 +1165,10 @@
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C5" s="5" t="n">
+        <f aca="false">COUNTIF(links!$A$1:$A$868, A5) &gt; 0</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -738,6 +1177,10 @@
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="C6" s="5" t="n">
+        <f aca="false">COUNTIF(links!$A$1:$A$868, A6) &gt; 0</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
@@ -746,6 +1189,10 @@
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="C7" s="5" t="n">
+        <f aca="false">COUNTIF(links!$A$1:$A$868, A7) &gt; 0</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
@@ -754,6 +1201,10 @@
       <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="C8" s="5" t="n">
+        <f aca="false">COUNTIF(links!$A$1:$A$868, A8) &gt; 0</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
@@ -762,6 +1213,10 @@
       <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="C9" s="5" t="n">
+        <f aca="false">COUNTIF(links!$A$1:$A$868, A9) &gt; 0</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
@@ -770,6 +1225,10 @@
       <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="C10" s="5" t="n">
+        <f aca="false">COUNTIF(links!$A$1:$A$868, A10) &gt; 0</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
@@ -778,6 +1237,10 @@
       <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="C11" s="5" t="n">
+        <f aca="false">COUNTIF(links!$A$1:$A$868, A11) &gt; 0</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
@@ -786,21 +1249,9 @@
       <c r="B12" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>27</v>
+      <c r="C12" s="5" t="n">
+        <f aca="false">COUNTIF(links!$A$1:$A$868, A12) &gt; 0</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -811,6 +1262,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -819,199 +1271,304 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.86"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="3" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="21" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="6" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="2" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="4" t="b">
+        <f aca="false">AND(E2:E832)</f>
+        <v>1</v>
+      </c>
+      <c r="F1" s="4" t="b">
+        <f aca="false">AND(F2:F832)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="23" t="n">
+        <v>100</v>
+      </c>
+      <c r="D2" s="23" t="n">
+        <v>200</v>
+      </c>
+      <c r="E2" s="5" t="b">
+        <f aca="false">COUNTIF(experts!$A$2:$A$985, A2) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="5" t="b">
+        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B2) &gt; 0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="23" t="n">
+        <v>100</v>
+      </c>
+      <c r="D3" s="23" t="n">
+        <v>200</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$985, A3) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B3) &gt; 0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="C4" s="23" t="n">
+        <v>100</v>
+      </c>
+      <c r="D4" s="23" t="n">
+        <v>200</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$985, A4) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B4) &gt; 0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="23" t="n">
+        <v>200</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$985, A5) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B5) &gt; 0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="19" t="n">
-        <v>100</v>
-      </c>
-      <c r="D2" s="19" t="n">
+      <c r="C6" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="23" t="n">
         <v>200</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="19" t="n">
-        <v>100</v>
-      </c>
-      <c r="D3" s="19" t="n">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" s="19" t="n">
-        <v>100</v>
-      </c>
-      <c r="D4" s="19" t="n">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="C5" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="19" t="n">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="C6" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" s="19" t="n">
-        <v>200</v>
+      <c r="E6" s="5" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$985, A6) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F6" s="5" t="n">
+        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B6) &gt; 0</f>
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="20" t="s">
-        <v>60</v>
+      <c r="B7" s="6" t="s">
+        <v>52</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>0</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>200</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$985, A7) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B7) &gt; 0</f>
+        <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="20" t="s">
-        <v>61</v>
+      <c r="B8" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>0</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>201</v>
+      </c>
+      <c r="E8" s="5" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$985, A8) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F8" s="5" t="n">
+        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B8) &gt; 0</f>
+        <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="21" t="s">
-        <v>62</v>
+      <c r="B9" s="24" t="s">
+        <v>54</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>0</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>202</v>
+      </c>
+      <c r="E9" s="5" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$985, A9) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F9" s="5" t="n">
+        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B9) &gt; 0</f>
+        <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="21" t="s">
-        <v>65</v>
+      <c r="B10" s="24" t="s">
+        <v>55</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>0</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>203</v>
+      </c>
+      <c r="E10" s="5" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$985, A10) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F10" s="5" t="n">
+        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B10) &gt; 0</f>
+        <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="21" t="s">
-        <v>68</v>
+      <c r="B11" s="24" t="s">
+        <v>56</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>0</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>204</v>
+      </c>
+      <c r="E11" s="5" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$985, A11) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F11" s="5" t="n">
+        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B11) &gt; 0</f>
+        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="21" t="s">
-        <v>71</v>
+      <c r="B12" s="24" t="s">
+        <v>57</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>0</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>205</v>
+      </c>
+      <c r="E12" s="5" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$985, A12) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F12" s="5" t="n">
+        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B12) &gt; 0</f>
+        <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="21" t="s">
-        <v>74</v>
+      <c r="B13" s="24" t="s">
+        <v>58</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>0</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>206</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$985, A13) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B13) &gt; 0</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1022,6 +1579,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1030,30 +1588,34 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
-        <v>78</v>
+      <c r="A1" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="10" t="b">
+        <f aca="false">AND(B2:B904)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14" t="n">
-        <v>45413</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="n">
+      <c r="A2" s="17" t="n">
         <v>45651</v>
+      </c>
+      <c r="B2" s="5" t="b">
+        <f aca="false">AND(ISNUMBER(A2),misc!$A$2&lt;=A2)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1064,6 +1626,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1072,68 +1635,104 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="19.48"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="19.48"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="3" style="25" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>86</v>
+      <c r="A1" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="L1" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="M1" s="26" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" s="3" t="n">
+      <c r="A2" s="17" t="n">
+        <v>45641</v>
+      </c>
+      <c r="B2" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="C2" s="22" t="n">
+      <c r="C2" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="D2" s="23" t="n">
+      <c r="D2" s="15" t="n">
         <v>45642</v>
       </c>
-      <c r="E2" s="23" t="n">
+      <c r="E2" s="15" t="n">
         <v>45778</v>
       </c>
-      <c r="F2" s="23" t="n">
+      <c r="F2" s="15" t="n">
         <v>45642</v>
       </c>
-      <c r="G2" s="23" t="n">
+      <c r="G2" s="15" t="n">
         <v>45778</v>
       </c>
-      <c r="H2" s="22" t="s">
-        <v>88</v>
+      <c r="H2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2" s="27" t="n">
+        <f aca="false">MAX(MAX('invoicing periods'!C2:C900),MAX(tasks!C2:C896))</f>
+        <v>45795</v>
+      </c>
+      <c r="J2" s="28" t="n">
+        <f aca="false">AND(ISNUMBER(D2), D2&gt;A2)</f>
+        <v>1</v>
+      </c>
+      <c r="K2" s="29" t="b">
+        <f aca="false">AND(ISNUMBER(E2), E2&lt;=I2)</f>
+        <v>1</v>
+      </c>
+      <c r="L2" s="29" t="b">
+        <f aca="false">AND(ISNUMBER(F2), F2&gt;A2)</f>
+        <v>1</v>
+      </c>
+      <c r="M2" s="29" t="b">
+        <f aca="false">AND(ISNUMBER(G2), G2&lt;=I2)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1152,380 +1751,589 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="3" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="6" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="5" style="2" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="10" t="b">
+        <f aca="false">AND(E2:E899)</f>
+        <v>1</v>
+      </c>
+      <c r="F1" s="10" t="b">
+        <f aca="false">AND(F2:F904)</f>
+        <v>1</v>
+      </c>
+      <c r="G1" s="10" t="b">
+        <f aca="false">AND(G2:G904)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="12" t="n">
+        <v>45642</v>
+      </c>
+      <c r="C2" s="12" t="n">
+        <v>45749</v>
+      </c>
+      <c r="D2" s="13" t="n">
+        <v>400</v>
+      </c>
+      <c r="E2" s="5" t="b">
+        <f aca="false">COUNTIF(links!$B$1:$B$868, A2) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="5" t="b">
+        <f aca="false">C2&gt;misc!$A$2</f>
+        <v>1</v>
+      </c>
+      <c r="G2" s="5" t="b">
+        <f aca="false">AND(ISNUMBER(B2), ISNUMBER(C2), B2&lt;=C2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="B3" s="12" t="n">
+        <v>45642</v>
+      </c>
+      <c r="C3" s="12" t="n">
+        <v>45749</v>
+      </c>
+      <c r="D3" s="13" t="n">
+        <v>420</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <f aca="false">COUNTIF(links!$B$1:$B$868, A3) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <f aca="false">C3&gt;misc!$A$2</f>
+        <v>1</v>
+      </c>
+      <c r="G3" s="5" t="n">
+        <f aca="false">AND(ISNUMBER(B3), ISNUMBER(C3), B3&lt;=C3)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="B4" s="12" t="n">
+        <v>45642</v>
+      </c>
+      <c r="C4" s="12" t="n">
+        <v>45749</v>
+      </c>
+      <c r="D4" s="13" t="n">
+        <v>430</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <f aca="false">COUNTIF(links!$B$1:$B$868, A4) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <f aca="false">C4&gt;misc!$A$2</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <f aca="false">AND(ISNUMBER(B4), ISNUMBER(C4), B4&lt;=C4)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="11" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+      <c r="B5" s="12" t="n">
+        <v>45642</v>
+      </c>
+      <c r="C5" s="12" t="n">
+        <v>45749</v>
+      </c>
+      <c r="D5" s="13" t="n">
+        <v>440</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <f aca="false">COUNTIF(links!$B$1:$B$868, A5) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <f aca="false">C5&gt;misc!$A$2</f>
+        <v>1</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <f aca="false">AND(ISNUMBER(B5), ISNUMBER(C5), B5&lt;=C5)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="8" t="n">
+      <c r="B6" s="12" t="n">
         <v>45642</v>
       </c>
-      <c r="C2" s="8" t="n">
+      <c r="C6" s="12" t="n">
+        <v>45718</v>
+      </c>
+      <c r="D6" s="13" t="n">
+        <v>200</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <f aca="false">COUNTIF(links!$B$1:$B$868, A6) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F6" s="5" t="n">
+        <f aca="false">C6&gt;misc!$A$2</f>
+        <v>1</v>
+      </c>
+      <c r="G6" s="5" t="n">
+        <f aca="false">AND(ISNUMBER(B6), ISNUMBER(C6), B6&lt;=C6)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="12" t="n">
+        <v>45642</v>
+      </c>
+      <c r="C7" s="12" t="n">
         <v>45749</v>
       </c>
-      <c r="D2" s="9" t="n">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="8" t="n">
+      <c r="D7" s="13" t="n">
+        <v>200</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <f aca="false">COUNTIF(links!$B$1:$B$868, A7) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <f aca="false">C7&gt;misc!$A$2</f>
+        <v>1</v>
+      </c>
+      <c r="G7" s="5" t="n">
+        <f aca="false">AND(ISNUMBER(B7), ISNUMBER(C7), B7&lt;=C7)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="12" t="n">
         <v>45642</v>
       </c>
-      <c r="C3" s="8" t="n">
+      <c r="C8" s="12" t="n">
+        <v>45718</v>
+      </c>
+      <c r="D8" s="13" t="n">
+        <v>200</v>
+      </c>
+      <c r="E8" s="5" t="n">
+        <f aca="false">COUNTIF(links!$B$1:$B$868, A8) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F8" s="5" t="n">
+        <f aca="false">C8&gt;misc!$A$2</f>
+        <v>1</v>
+      </c>
+      <c r="G8" s="5" t="n">
+        <f aca="false">AND(ISNUMBER(B8), ISNUMBER(C8), B8&lt;=C8)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="12" t="n">
+        <v>45642</v>
+      </c>
+      <c r="C9" s="12" t="n">
         <v>45749</v>
       </c>
-      <c r="D3" s="9" t="n">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="8" t="n">
+      <c r="D9" s="13" t="n">
+        <v>200</v>
+      </c>
+      <c r="E9" s="5" t="n">
+        <f aca="false">COUNTIF(links!$B$1:$B$868, A9) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F9" s="5" t="n">
+        <f aca="false">C9&gt;misc!$A$2</f>
+        <v>1</v>
+      </c>
+      <c r="G9" s="5" t="n">
+        <f aca="false">AND(ISNUMBER(B9), ISNUMBER(C9), B9&lt;=C9)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="12" t="n">
         <v>45642</v>
       </c>
-      <c r="C4" s="8" t="n">
+      <c r="C10" s="12" t="n">
+        <v>45718</v>
+      </c>
+      <c r="D10" s="13" t="n">
+        <v>200</v>
+      </c>
+      <c r="E10" s="5" t="n">
+        <f aca="false">COUNTIF(links!$B$1:$B$868, A10) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F10" s="5" t="n">
+        <f aca="false">C10&gt;misc!$A$2</f>
+        <v>1</v>
+      </c>
+      <c r="G10" s="5" t="n">
+        <f aca="false">AND(ISNUMBER(B10), ISNUMBER(C10), B10&lt;=C10)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="12" t="n">
+        <v>45642</v>
+      </c>
+      <c r="C11" s="12" t="n">
         <v>45749</v>
       </c>
-      <c r="D4" s="9" t="n">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="8" t="n">
+      <c r="D11" s="13" t="n">
+        <v>200</v>
+      </c>
+      <c r="E11" s="5" t="n">
+        <f aca="false">COUNTIF(links!$B$1:$B$868, A11) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F11" s="5" t="n">
+        <f aca="false">C11&gt;misc!$A$2</f>
+        <v>1</v>
+      </c>
+      <c r="G11" s="5" t="n">
+        <f aca="false">AND(ISNUMBER(B11), ISNUMBER(C11), B11&lt;=C11)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="12" t="n">
         <v>45642</v>
       </c>
-      <c r="C5" s="8" t="n">
+      <c r="C12" s="12" t="n">
+        <v>45718</v>
+      </c>
+      <c r="D12" s="13" t="n">
+        <v>200</v>
+      </c>
+      <c r="E12" s="5" t="n">
+        <f aca="false">COUNTIF(links!$B$1:$B$868, A12) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F12" s="5" t="n">
+        <f aca="false">C12&gt;misc!$A$2</f>
+        <v>1</v>
+      </c>
+      <c r="G12" s="5" t="n">
+        <f aca="false">AND(ISNUMBER(B12), ISNUMBER(C12), B12&lt;=C12)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="12" t="n">
+        <v>45642</v>
+      </c>
+      <c r="C13" s="12" t="n">
         <v>45749</v>
       </c>
-      <c r="D5" s="9" t="n">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="8" t="n">
+      <c r="D13" s="13" t="n">
+        <v>200</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <f aca="false">COUNTIF(links!$B$1:$B$868, A13) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <f aca="false">C13&gt;misc!$A$2</f>
+        <v>1</v>
+      </c>
+      <c r="G13" s="5" t="n">
+        <f aca="false">AND(ISNUMBER(B13), ISNUMBER(C13), B13&lt;=C13)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="12" t="n">
         <v>45642</v>
       </c>
-      <c r="C6" s="8" t="n">
+      <c r="C14" s="12" t="n">
         <v>45718</v>
       </c>
-      <c r="D6" s="9" t="n">
+      <c r="D14" s="13" t="n">
         <v>200</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="8" t="n">
+      <c r="E14" s="5" t="n">
+        <f aca="false">COUNTIF(links!$B$1:$B$868, A14) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <f aca="false">C14&gt;misc!$A$2</f>
+        <v>1</v>
+      </c>
+      <c r="G14" s="5" t="n">
+        <f aca="false">AND(ISNUMBER(B14), ISNUMBER(C14), B14&lt;=C14)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="12" t="n">
         <v>45642</v>
       </c>
-      <c r="C7" s="8" t="n">
+      <c r="C15" s="12" t="n">
         <v>45749</v>
       </c>
-      <c r="D7" s="9" t="n">
+      <c r="D15" s="13" t="n">
         <v>200</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="8" t="n">
+      <c r="E15" s="5" t="n">
+        <f aca="false">COUNTIF(links!$B$1:$B$868, A15) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F15" s="5" t="n">
+        <f aca="false">C15&gt;misc!$A$2</f>
+        <v>1</v>
+      </c>
+      <c r="G15" s="5" t="n">
+        <f aca="false">AND(ISNUMBER(B15), ISNUMBER(C15), B15&lt;=C15)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="12" t="n">
         <v>45642</v>
       </c>
-      <c r="C8" s="8" t="n">
+      <c r="C16" s="12" t="n">
+        <v>45779</v>
+      </c>
+      <c r="D16" s="13" t="n">
+        <v>200</v>
+      </c>
+      <c r="E16" s="5" t="n">
+        <f aca="false">COUNTIF(links!$B$1:$B$868, A16) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F16" s="5" t="n">
+        <f aca="false">C16&gt;misc!$A$2</f>
+        <v>1</v>
+      </c>
+      <c r="G16" s="5" t="n">
+        <f aca="false">AND(ISNUMBER(B16), ISNUMBER(C16), B16&lt;=C16)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="12" t="n">
+        <v>45642</v>
+      </c>
+      <c r="C17" s="12" t="n">
         <v>45718</v>
       </c>
-      <c r="D8" s="9" t="n">
+      <c r="D17" s="13" t="n">
         <v>200</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="8" t="n">
+      <c r="E17" s="5" t="n">
+        <f aca="false">COUNTIF(links!$B$1:$B$868, A17) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F17" s="5" t="n">
+        <f aca="false">C17&gt;misc!$A$2</f>
+        <v>1</v>
+      </c>
+      <c r="G17" s="5" t="n">
+        <f aca="false">AND(ISNUMBER(B17), ISNUMBER(C17), B17&lt;=C17)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="12" t="n">
         <v>45642</v>
       </c>
-      <c r="C9" s="8" t="n">
+      <c r="C18" s="12" t="n">
         <v>45749</v>
       </c>
-      <c r="D9" s="9" t="n">
+      <c r="D18" s="13" t="n">
         <v>200</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="8" t="n">
+      <c r="E18" s="5" t="n">
+        <f aca="false">COUNTIF(links!$B$1:$B$868, A18) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F18" s="5" t="n">
+        <f aca="false">C18&gt;misc!$A$2</f>
+        <v>1</v>
+      </c>
+      <c r="G18" s="5" t="n">
+        <f aca="false">AND(ISNUMBER(B18), ISNUMBER(C18), B18&lt;=C18)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="12" t="n">
         <v>45642</v>
       </c>
-      <c r="C10" s="8" t="n">
+      <c r="C19" s="12" t="n">
+        <v>45779</v>
+      </c>
+      <c r="D19" s="13" t="n">
+        <v>200</v>
+      </c>
+      <c r="E19" s="5" t="n">
+        <f aca="false">COUNTIF(links!$B$1:$B$868, A19) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F19" s="5" t="n">
+        <f aca="false">C19&gt;misc!$A$2</f>
+        <v>1</v>
+      </c>
+      <c r="G19" s="5" t="n">
+        <f aca="false">AND(ISNUMBER(B19), ISNUMBER(C19), B19&lt;=C19)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="12" t="n">
+        <v>45642</v>
+      </c>
+      <c r="C20" s="12" t="n">
         <v>45718</v>
       </c>
-      <c r="D10" s="9" t="n">
+      <c r="D20" s="13" t="n">
         <v>200</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="8" t="n">
+      <c r="E20" s="5" t="n">
+        <f aca="false">COUNTIF(links!$B$1:$B$868, A20) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F20" s="5" t="n">
+        <f aca="false">C20&gt;misc!$A$2</f>
+        <v>1</v>
+      </c>
+      <c r="G20" s="5" t="n">
+        <f aca="false">AND(ISNUMBER(B20), ISNUMBER(C20), B20&lt;=C20)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="12" t="n">
         <v>45642</v>
       </c>
-      <c r="C11" s="8" t="n">
+      <c r="C21" s="12" t="n">
         <v>45749</v>
       </c>
-      <c r="D11" s="9" t="n">
+      <c r="D21" s="13" t="n">
         <v>200</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="8" t="n">
+      <c r="E21" s="5" t="n">
+        <f aca="false">COUNTIF(links!$B$1:$B$868, A21) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F21" s="5" t="n">
+        <f aca="false">C21&gt;misc!$A$2</f>
+        <v>1</v>
+      </c>
+      <c r="G21" s="5" t="n">
+        <f aca="false">AND(ISNUMBER(B21), ISNUMBER(C21), B21&lt;=C21)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="12" t="n">
         <v>45642</v>
       </c>
-      <c r="C12" s="8" t="n">
-        <v>45718</v>
-      </c>
-      <c r="D12" s="9" t="n">
+      <c r="C22" s="12" t="n">
+        <v>45779</v>
+      </c>
+      <c r="D22" s="13" t="n">
         <v>200</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="8" t="n">
-        <v>45642</v>
-      </c>
-      <c r="C13" s="8" t="n">
-        <v>45749</v>
-      </c>
-      <c r="D13" s="9" t="n">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="8" t="n">
-        <v>45642</v>
-      </c>
-      <c r="C14" s="8" t="n">
-        <v>45718</v>
-      </c>
-      <c r="D14" s="9" t="n">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" s="8" t="n">
-        <v>45642</v>
-      </c>
-      <c r="C15" s="8" t="n">
-        <v>45749</v>
-      </c>
-      <c r="D15" s="9" t="n">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" s="8" t="n">
-        <v>45642</v>
-      </c>
-      <c r="C16" s="8" t="n">
-        <v>45779</v>
-      </c>
-      <c r="D16" s="9" t="n">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" s="8" t="n">
-        <v>45642</v>
-      </c>
-      <c r="C17" s="8" t="n">
-        <v>45718</v>
-      </c>
-      <c r="D17" s="9" t="n">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="8" t="n">
-        <v>45642</v>
-      </c>
-      <c r="C18" s="8" t="n">
-        <v>45749</v>
-      </c>
-      <c r="D18" s="9" t="n">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" s="8" t="n">
-        <v>45642</v>
-      </c>
-      <c r="C19" s="8" t="n">
-        <v>45779</v>
-      </c>
-      <c r="D19" s="9" t="n">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" s="8" t="n">
-        <v>45642</v>
-      </c>
-      <c r="C20" s="8" t="n">
-        <v>45718</v>
-      </c>
-      <c r="D20" s="9" t="n">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="8" t="n">
-        <v>45642</v>
-      </c>
-      <c r="C21" s="8" t="n">
-        <v>45749</v>
-      </c>
-      <c r="D21" s="9" t="n">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B22" s="8" t="n">
-        <v>45642</v>
-      </c>
-      <c r="C22" s="8" t="n">
-        <v>45779</v>
-      </c>
-      <c r="D22" s="9" t="n">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B23" s="10" t="n">
-        <v>45292</v>
-      </c>
-      <c r="C23" s="10" t="n">
-        <v>45324</v>
-      </c>
-      <c r="D23" s="3" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B24" s="10" t="n">
-        <v>45352</v>
-      </c>
-      <c r="C24" s="10" t="n">
-        <v>45384</v>
-      </c>
-      <c r="D24" s="3" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B25" s="10" t="n">
-        <v>45383</v>
-      </c>
-      <c r="C25" s="10" t="n">
-        <v>45414</v>
-      </c>
-      <c r="D25" s="3" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B26" s="10" t="n">
-        <v>45658</v>
-      </c>
-      <c r="C26" s="10" t="n">
-        <v>45751</v>
-      </c>
-      <c r="D26" s="3" t="n">
-        <v>70</v>
+      <c r="E22" s="5" t="n">
+        <f aca="false">COUNTIF(links!$B$1:$B$868, A22) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <f aca="false">C22&gt;misc!$A$2</f>
+        <v>1</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <f aca="false">AND(ISNUMBER(B22), ISNUMBER(C22), B22&lt;=C22)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1536,6 +2344,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1544,24 +2353,33 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.76"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="2" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>57</v>
+      <c r="A1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="4" t="b">
+        <f aca="false">AND(C2:C933)</f>
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="b">
+        <f aca="false">AND(D2:D933)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1569,7 +2387,15 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
+      </c>
+      <c r="C2" s="14" t="b">
+        <f aca="false">COUNTIF(experts!$A$2:$A$986, A2) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="D2" s="14" t="b">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903, B2) &gt; 0</f>
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1577,7 +2403,15 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
+      </c>
+      <c r="C3" s="14" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$986, A3) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="D3" s="14" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903, B3) &gt; 0</f>
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1585,7 +2419,15 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+      <c r="C4" s="14" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$986, A4) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="D4" s="14" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903, B4) &gt; 0</f>
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1593,7 +2435,15 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
+      </c>
+      <c r="C5" s="14" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$986, A5) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="D5" s="14" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903, B5) &gt; 0</f>
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1601,7 +2451,15 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
+      </c>
+      <c r="C6" s="14" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$986, A6) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="D6" s="14" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903, B6) &gt; 0</f>
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1609,7 +2467,15 @@
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
+      </c>
+      <c r="C7" s="14" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$986, A7) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="D7" s="14" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903, B7) &gt; 0</f>
+        <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1617,7 +2483,15 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
+      </c>
+      <c r="C8" s="14" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$986, A8) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="D8" s="14" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903, B8) &gt; 0</f>
+        <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1625,7 +2499,15 @@
         <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
+      </c>
+      <c r="C9" s="14" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$986, A9) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="D9" s="14" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903, B9) &gt; 0</f>
+        <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1633,7 +2515,15 @@
         <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
+      </c>
+      <c r="C10" s="14" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$986, A10) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="D10" s="14" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903, B10) &gt; 0</f>
+        <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1641,7 +2531,15 @@
         <v>14</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
+      </c>
+      <c r="C11" s="14" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$986, A11) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="D11" s="14" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903, B11) &gt; 0</f>
+        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1649,7 +2547,15 @@
         <v>16</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
+      </c>
+      <c r="C12" s="14" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$986, A12) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="D12" s="14" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903, B12) &gt; 0</f>
+        <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1657,7 +2563,15 @@
         <v>16</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
+      </c>
+      <c r="C13" s="14" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$986, A13) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="D13" s="14" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903, B13) &gt; 0</f>
+        <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1665,7 +2579,15 @@
         <v>18</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
+      </c>
+      <c r="C14" s="14" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$986, A14) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="D14" s="14" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903, B14) &gt; 0</f>
+        <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1673,7 +2595,15 @@
         <v>18</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
+      </c>
+      <c r="C15" s="14" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$986, A15) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="D15" s="14" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903, B15) &gt; 0</f>
+        <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1681,7 +2611,15 @@
         <v>18</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
+      </c>
+      <c r="C16" s="14" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$986, A16) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="D16" s="14" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903, B16) &gt; 0</f>
+        <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1689,7 +2627,15 @@
         <v>20</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
+      </c>
+      <c r="C17" s="14" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$986, A17) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="D17" s="14" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903, B17) &gt; 0</f>
+        <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1697,7 +2643,15 @@
         <v>20</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
+      </c>
+      <c r="C18" s="14" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$986, A18) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="D18" s="14" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903, B18) &gt; 0</f>
+        <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1705,7 +2659,15 @@
         <v>20</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
+      </c>
+      <c r="C19" s="14" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$986, A19) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="D19" s="14" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903, B19) &gt; 0</f>
+        <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1713,7 +2675,15 @@
         <v>22</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
+      </c>
+      <c r="C20" s="14" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$986, A20) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="D20" s="14" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903, B20) &gt; 0</f>
+        <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1721,7 +2691,15 @@
         <v>22</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="C21" s="14" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$986, A21) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="D21" s="14" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903, B21) &gt; 0</f>
+        <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1729,31 +2707,15 @@
         <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
+      </c>
+      <c r="C22" s="14" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$986, A22) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="D22" s="14" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903, B22) &gt; 0</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1764,6 +2726,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1772,37 +2735,50 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F70"/>
+  <dimension ref="A1:I67"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.76"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="3" style="3" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="3" style="6" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="7" style="2" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>59</v>
+      <c r="A1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="4" t="b">
+        <f aca="false">AND(G2:G934)</f>
+        <v>1</v>
+      </c>
+      <c r="H1" s="4" t="b">
+        <f aca="false">AND(H2:H934)</f>
+        <v>1</v>
+      </c>
+      <c r="I1" s="10" t="b">
+        <f aca="false">AND(I2:I904)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1810,12 +2786,12 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="11" t="n">
+        <v>28</v>
+      </c>
+      <c r="C2" s="15" t="n">
         <v>45642</v>
       </c>
-      <c r="D2" s="11" t="n">
+      <c r="D2" s="15" t="n">
         <v>45653</v>
       </c>
       <c r="E2" s="1" t="n">
@@ -1824,106 +2800,100 @@
       <c r="F2" s="1" t="n">
         <v>6</v>
       </c>
+      <c r="G2" s="14" t="b">
+        <f aca="false">COUNTIF(experts!$A$2:$A$986, A2) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H2" s="14" t="b">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903,B2)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="I2" s="5" t="b">
+        <f aca="false">AND(ISNUMBER(C2), ISNUMBER(D2), C2&lt;=D2)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="12" t="n">
+      <c r="B3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="16" t="n">
         <v>45642</v>
       </c>
-      <c r="D3" s="12" t="n">
+      <c r="D3" s="16" t="n">
         <v>45646</v>
       </c>
-      <c r="E3" s="7" t="n">
+      <c r="E3" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="F3" s="7" t="n">
+      <c r="F3" s="11" t="n">
         <v>5</v>
       </c>
+      <c r="G3" s="14" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$986, A3) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H3" s="14" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903,B3)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="I3" s="5" t="n">
+        <f aca="false">AND(ISNUMBER(C3), ISNUMBER(D3), C3&lt;=D3)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="12" t="n">
+      <c r="B4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="16" t="n">
         <v>45649</v>
       </c>
-      <c r="D4" s="12" t="n">
+      <c r="D4" s="16" t="n">
         <v>45653</v>
       </c>
-      <c r="E4" s="7" t="n">
+      <c r="E4" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="F4" s="7" t="n">
+      <c r="F4" s="11" t="n">
         <v>3</v>
       </c>
+      <c r="G4" s="14" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$986, A4) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H4" s="14" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903,B4)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="I4" s="5" t="n">
+        <f aca="false">AND(ISNUMBER(C4), ISNUMBER(D4), C4&lt;=D4)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="10" t="n">
-        <v>45292</v>
-      </c>
-      <c r="D5" s="10" t="n">
-        <v>45324</v>
-      </c>
-      <c r="E5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1" t="n">
-        <v>2</v>
-      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="10" t="n">
-        <v>45352</v>
-      </c>
-      <c r="D6" s="10" t="n">
-        <v>45384</v>
-      </c>
-      <c r="E6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1" t="n">
-        <v>2</v>
-      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="10" t="n">
-        <v>45383</v>
-      </c>
-      <c r="D7" s="10" t="n">
-        <v>45414</v>
-      </c>
-      <c r="E7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1" t="n">
-        <v>2</v>
-      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="1"/>
@@ -2284,24 +3254,6 @@
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
-      <c r="E68" s="1"/>
-      <c r="F68" s="1"/>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
-    </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2311,6 +3263,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2319,38 +3272,51 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F70"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.76"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="3" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="6" width="11.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="7" style="2" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>59</v>
+      <c r="A1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="4" t="b">
+        <f aca="false">AND(G2:G938)</f>
+        <v>1</v>
+      </c>
+      <c r="H1" s="4" t="b">
+        <f aca="false">AND(H2:H938)</f>
+        <v>1</v>
+      </c>
+      <c r="I1" s="10" t="b">
+        <f aca="false">AND(I2:I908)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2358,12 +3324,12 @@
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="11" t="n">
+        <v>30</v>
+      </c>
+      <c r="C2" s="15" t="n">
         <v>45642</v>
       </c>
-      <c r="D2" s="11" t="n">
+      <c r="D2" s="15" t="n">
         <v>45646</v>
       </c>
       <c r="E2" s="1" t="n">
@@ -2372,66 +3338,42 @@
       <c r="F2" s="1" t="n">
         <v>16</v>
       </c>
+      <c r="G2" s="5" t="b">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A2) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H2" s="5" t="b">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903,B2)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="I2" s="5" t="b">
+        <f aca="false">AND(ISNUMBER(C2), ISNUMBER(D2), C2&lt;=D2)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="10" t="n">
-        <v>45292</v>
-      </c>
-      <c r="D3" s="10" t="n">
-        <v>45296</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1" t="n">
-        <v>20</v>
-      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="1"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="10" t="n">
-        <v>45352</v>
-      </c>
-      <c r="D4" s="10" t="n">
-        <v>45361</v>
-      </c>
-      <c r="E4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1" t="n">
-        <v>15</v>
-      </c>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="1"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="10" t="n">
-        <v>45383</v>
-      </c>
-      <c r="D5" s="10" t="n">
-        <v>45389</v>
-      </c>
-      <c r="E5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1" t="n">
-        <v>13</v>
-      </c>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="1"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="1"/>
@@ -2766,6 +3708,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2774,43 +3717,52 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.76"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="2" style="3" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="2" style="6" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="6" style="2" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>59</v>
+      <c r="A1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="4" t="b">
+        <f aca="false">AND(F2:F935)</f>
+        <v>1</v>
+      </c>
+      <c r="G1" s="10" t="b">
+        <f aca="false">AND(G2:G905)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="11" t="n">
+      <c r="B2" s="15" t="n">
         <v>45642</v>
       </c>
-      <c r="C2" s="11" t="n">
+      <c r="C2" s="15" t="n">
         <v>45653</v>
       </c>
       <c r="D2" s="1" t="n">
@@ -2818,22 +3770,38 @@
       </c>
       <c r="E2" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="F2" s="5" t="b">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987,A2)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="G2" s="5" t="b">
+        <f aca="false">AND(ISNUMBER(B2), ISNUMBER(C2), B2&lt;=C2)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="11" t="n">
+      <c r="B3" s="15" t="n">
         <v>45642</v>
       </c>
-      <c r="C3" s="11" t="n">
+      <c r="C3" s="15" t="n">
         <v>45653</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987,A3)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="G3" s="5" t="n">
+        <f aca="false">AND(ISNUMBER(B3), ISNUMBER(C3), B3&lt;=C3)</f>
         <v>1</v>
       </c>
     </row>
@@ -2841,10 +3809,10 @@
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="11" t="n">
+      <c r="B4" s="15" t="n">
         <v>45642</v>
       </c>
-      <c r="C4" s="11" t="n">
+      <c r="C4" s="15" t="n">
         <v>45653</v>
       </c>
       <c r="D4" s="1" t="n">
@@ -2852,16 +3820,24 @@
       </c>
       <c r="E4" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987,A4)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <f aca="false">AND(ISNUMBER(B4), ISNUMBER(C4), B4&lt;=C4)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="11" t="n">
+      <c r="B5" s="15" t="n">
         <v>45642</v>
       </c>
-      <c r="C5" s="11" t="n">
+      <c r="C5" s="15" t="n">
         <v>45653</v>
       </c>
       <c r="D5" s="1" t="n">
@@ -2870,57 +3846,38 @@
       <c r="E5" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="F5" s="5" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987,A5)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <f aca="false">AND(ISNUMBER(B5), ISNUMBER(C5), B5&lt;=C5)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="10" t="n">
-        <v>45292</v>
-      </c>
-      <c r="C6" s="10" t="n">
-        <v>45324</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1" t="n">
-        <v>2</v>
-      </c>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="10" t="n">
-        <v>45352</v>
-      </c>
-      <c r="C7" s="10" t="n">
-        <v>45384</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1" t="n">
-        <v>2</v>
-      </c>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="10" t="n">
-        <v>45383</v>
-      </c>
-      <c r="C8" s="10" t="n">
-        <v>45414</v>
-      </c>
-      <c r="D8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1" t="n">
-        <v>2</v>
-      </c>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1"/>
@@ -3302,6 +4259,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3310,38 +4268,51 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F70"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.76"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="3" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="6" width="11.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="7" style="2" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>59</v>
+      <c r="A1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="4" t="b">
+        <f aca="false">AND(G2:G938)</f>
+        <v>1</v>
+      </c>
+      <c r="H1" s="4" t="b">
+        <f aca="false">AND(H2:H938)</f>
+        <v>1</v>
+      </c>
+      <c r="I1" s="10" t="b">
+        <f aca="false">AND(I2:I908)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3349,12 +4320,12 @@
         <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="11" t="n">
+        <v>35</v>
+      </c>
+      <c r="C2" s="15" t="n">
         <v>45642</v>
       </c>
-      <c r="D2" s="11" t="n">
+      <c r="D2" s="15" t="n">
         <v>45646</v>
       </c>
       <c r="E2" s="1" t="n">
@@ -3362,6 +4333,18 @@
       </c>
       <c r="F2" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="G2" s="5" t="b">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A2) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H2" s="5" t="b">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903,B2)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="I2" s="5" t="b">
+        <f aca="false">AND(ISNUMBER(C2), ISNUMBER(D2), C2&lt;=D2)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3369,12 +4352,12 @@
         <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="11" t="n">
+        <v>37</v>
+      </c>
+      <c r="C3" s="15" t="n">
         <v>45642</v>
       </c>
-      <c r="D3" s="11" t="n">
+      <c r="D3" s="15" t="n">
         <v>45646</v>
       </c>
       <c r="E3" s="1" t="n">
@@ -3382,6 +4365,18 @@
       </c>
       <c r="F3" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="G3" s="5" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A3) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H3" s="5" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903,B3)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="I3" s="5" t="n">
+        <f aca="false">AND(ISNUMBER(C3), ISNUMBER(D3), C3&lt;=D3)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3389,12 +4384,12 @@
         <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="11" t="n">
+        <v>42</v>
+      </c>
+      <c r="C4" s="15" t="n">
         <v>45642</v>
       </c>
-      <c r="D4" s="11" t="n">
+      <c r="D4" s="15" t="n">
         <v>45646</v>
       </c>
       <c r="E4" s="1" t="n">
@@ -3402,6 +4397,18 @@
       </c>
       <c r="F4" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A4) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H4" s="5" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903,B4)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="I4" s="5" t="n">
+        <f aca="false">AND(ISNUMBER(C4), ISNUMBER(D4), C4&lt;=D4)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3409,12 +4416,12 @@
         <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5" s="11" t="n">
+        <v>44</v>
+      </c>
+      <c r="C5" s="15" t="n">
         <v>45642</v>
       </c>
-      <c r="D5" s="11" t="n">
+      <c r="D5" s="15" t="n">
         <v>45646</v>
       </c>
       <c r="E5" s="1" t="n">
@@ -3422,6 +4429,18 @@
       </c>
       <c r="F5" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A5) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H5" s="5" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903,B5)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="I5" s="5" t="n">
+        <f aca="false">AND(ISNUMBER(C5), ISNUMBER(D5), C5&lt;=D5)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3429,12 +4448,12 @@
         <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="11" t="n">
+        <v>45</v>
+      </c>
+      <c r="C6" s="15" t="n">
         <v>45642</v>
       </c>
-      <c r="D6" s="11" t="n">
+      <c r="D6" s="15" t="n">
         <v>45646</v>
       </c>
       <c r="E6" s="1" t="n">
@@ -3443,26 +4462,26 @@
       <c r="F6" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="G6" s="5" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A6) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H6" s="5" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903,B6)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="I6" s="5" t="n">
+        <f aca="false">AND(ISNUMBER(C6), ISNUMBER(D6), C6&lt;=D6)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="10" t="n">
-        <v>45292</v>
-      </c>
-      <c r="D7" s="10" t="n">
-        <v>45324</v>
-      </c>
-      <c r="E7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1" t="n">
-        <v>3</v>
-      </c>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="1"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="1"/>
@@ -3787,6 +4806,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3795,199 +4815,229 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="2" style="3" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="2" style="6" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="6" style="2" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>59</v>
+      <c r="A1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="4" t="b">
+        <f aca="false">AND(F2:F938)</f>
+        <v>1</v>
+      </c>
+      <c r="G1" s="10" t="b">
+        <f aca="false">AND(G2:G908)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="10" t="n">
-        <v>45292</v>
-      </c>
-      <c r="C2" s="10" t="n">
-        <v>45301</v>
-      </c>
-      <c r="D2" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" s="15" t="n">
+        <v>45642</v>
+      </c>
+      <c r="C2" s="15" t="n">
+        <v>45689</v>
+      </c>
+      <c r="D2" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="E2" s="3" t="n">
-        <v>3</v>
+      <c r="E2" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2" s="5" t="b">
+        <f aca="false">COUNTIF(experts!$A$2:$A$985, A2) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="G2" s="5" t="b">
+        <f aca="false">AND(ISNUMBER(B2), ISNUMBER(C2), B2&lt;=C2)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="15" t="n">
+        <v>45690</v>
+      </c>
+      <c r="C3" s="15" t="n">
+        <v>45717</v>
+      </c>
+      <c r="D3" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="6" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3997,6 +5047,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4005,109 +5056,142 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="3" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="17" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>29</v>
+      <c r="B1" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="10" t="b">
+        <f aca="false">AND(D2:D908)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" s="14" t="n">
+      <c r="A2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="15" t="n">
         <v>45597</v>
       </c>
-      <c r="C2" s="14" t="n">
+      <c r="C2" s="15" t="n">
         <v>45626</v>
       </c>
+      <c r="D2" s="5" t="b">
+        <f aca="false">AND(ISNUMBER(B2), ISNUMBER(C2), B2&lt;=C2)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="B3" s="14" t="n">
+      <c r="A3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="15" t="n">
         <v>45627</v>
       </c>
-      <c r="C3" s="14" t="n">
+      <c r="C3" s="15" t="n">
         <v>45636</v>
       </c>
+      <c r="D3" s="5" t="n">
+        <f aca="false">AND(ISNUMBER(B3), ISNUMBER(C3), B3&lt;=C3)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>64</v>
+      <c r="A4" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="20" t="n">
+        <v>45637</v>
+      </c>
+      <c r="C4" s="20" t="n">
+        <v>45672</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <f aca="false">AND(ISNUMBER(B4), ISNUMBER(C4), B4&lt;=C4)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>67</v>
+      <c r="A5" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="20" t="n">
+        <v>45673</v>
+      </c>
+      <c r="C5" s="20" t="n">
+        <v>45701</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <f aca="false">AND(ISNUMBER(B5), ISNUMBER(C5), B5&lt;=C5)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>70</v>
+      <c r="A6" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="20" t="n">
+        <v>45702</v>
+      </c>
+      <c r="C6" s="20" t="n">
+        <v>45732</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <f aca="false">AND(ISNUMBER(B6), ISNUMBER(C6), B6&lt;=C6)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>73</v>
+      <c r="A7" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="20" t="n">
+        <v>45733</v>
+      </c>
+      <c r="C7" s="20" t="n">
+        <v>45761</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <f aca="false">AND(ISNUMBER(B7), ISNUMBER(C7), B7&lt;=C7)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>76</v>
+      <c r="A8" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="20" t="n">
+        <v>45762</v>
+      </c>
+      <c r="C8" s="20" t="n">
+        <v>45795</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <f aca="false">AND(ISNUMBER(B8), ISNUMBER(C8), B8&lt;=C8)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4117,5 +5201,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix problem in example 08
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/08-various-bounds/08-various-bounds.xlsx
+++ b/ampl-data-input-excel/08-various-bounds/08-various-bounds.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="experts" sheetId="1" state="visible" r:id="rId3"/>
@@ -43,7 +43,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Has Expert any task?</t>
         </r>
@@ -66,7 +65,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Valid expert?</t>
         </r>
@@ -79,7 +77,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Valid period?</t>
         </r>
@@ -102,7 +99,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Are dates OK?</t>
         </r>
@@ -125,7 +121,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Is task assign to an Expert?</t>
         </r>
@@ -138,7 +133,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Should task be included?</t>
         </r>
@@ -151,7 +145,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Are date OK?</t>
         </r>
@@ -174,7 +167,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Valid expert?</t>
         </r>
@@ -187,7 +179,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Valid task?</t>
         </r>
@@ -210,7 +201,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Valid expert?</t>
         </r>
@@ -223,7 +213,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Valid task?</t>
         </r>
@@ -236,7 +225,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Are date OK?</t>
         </r>
@@ -259,7 +247,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Valid expert?</t>
         </r>
@@ -272,7 +259,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Valid task?</t>
         </r>
@@ -285,7 +271,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Are date OK?</t>
         </r>
@@ -308,7 +293,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Valid expert?</t>
         </r>
@@ -321,7 +305,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Are date OK?</t>
         </r>
@@ -344,7 +327,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Valid expert?</t>
         </r>
@@ -357,7 +339,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Valid task?</t>
         </r>
@@ -370,7 +351,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Are date OK?</t>
         </r>
@@ -393,7 +373,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Valid expert?</t>
         </r>
@@ -406,7 +385,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Are date OK?</t>
         </r>
@@ -429,9 +407,8 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Are date OK?</t>
+          <t xml:space="preserve">Are dates OK?</t>
         </r>
       </text>
     </comment>
@@ -440,7 +417,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="73">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -596,12 +573,6 @@
   </si>
   <si>
     <t xml:space="preserve">Upper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24.Nov</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24.Dec</t>
   </si>
   <si>
     <t xml:space="preserve">25.Jan</t>
@@ -677,7 +648,7 @@
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -711,6 +682,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -793,7 +769,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -802,7 +778,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -811,10 +787,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -834,7 +806,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -892,10 +864,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -1129,7 +1097,7 @@
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5" t="b">
+      <c r="C2" s="2" t="b">
         <f aca="false">COUNTIF(links!$A$1:$A$868, A2) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1141,7 +1109,7 @@
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="5" t="n">
+      <c r="C3" s="2" t="n">
         <f aca="false">COUNTIF(links!$A$1:$A$868, A3) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1153,7 +1121,7 @@
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="5" t="n">
+      <c r="C4" s="2" t="n">
         <f aca="false">COUNTIF(links!$A$1:$A$868, A4) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1165,7 +1133,7 @@
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="5" t="n">
+      <c r="C5" s="2" t="n">
         <f aca="false">COUNTIF(links!$A$1:$A$868, A5) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1177,7 +1145,7 @@
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="5" t="n">
+      <c r="C6" s="2" t="n">
         <f aca="false">COUNTIF(links!$A$1:$A$868, A6) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1189,7 +1157,7 @@
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="5" t="n">
+      <c r="C7" s="2" t="n">
         <f aca="false">COUNTIF(links!$A$1:$A$868, A7) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1201,7 +1169,7 @@
       <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="5" t="n">
+      <c r="C8" s="2" t="n">
         <f aca="false">COUNTIF(links!$A$1:$A$868, A8) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1213,7 +1181,7 @@
       <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="5" t="n">
+      <c r="C9" s="2" t="n">
         <f aca="false">COUNTIF(links!$A$1:$A$868, A9) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1225,7 +1193,7 @@
       <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="5" t="n">
+      <c r="C10" s="2" t="n">
         <f aca="false">COUNTIF(links!$A$1:$A$868, A10) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1237,7 +1205,7 @@
       <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="5" t="n">
+      <c r="C11" s="2" t="n">
         <f aca="false">COUNTIF(links!$A$1:$A$868, A11) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1249,7 +1217,7 @@
       <c r="B12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="5" t="n">
+      <c r="C12" s="2" t="n">
         <f aca="false">COUNTIF(links!$A$1:$A$868, A12) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1271,149 +1239,149 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.86"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="21" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="6" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="5" width="11.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="2" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" s="8" t="s">
+      <c r="B1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E1" s="4" t="b">
-        <f aca="false">AND(E2:E832)</f>
+        <f aca="false">AND(E2:E830)</f>
         <v>1</v>
       </c>
       <c r="F1" s="4" t="b">
-        <f aca="false">AND(F2:F832)</f>
+        <f aca="false">AND(F2:F830)</f>
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="22" t="n">
+        <v>100</v>
+      </c>
+      <c r="D2" s="22" t="n">
+        <v>200</v>
+      </c>
+      <c r="E2" s="2" t="b">
+        <f aca="false">COUNTIF(experts!$A$2:$A$985, A2) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="2" t="b">
+        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$998, B2) &gt; 0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="22" t="n">
+        <v>100</v>
+      </c>
+      <c r="D3" s="22" t="n">
+        <v>200</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$985, A3) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="2" t="b">
+        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$998, B3) &gt; 0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="23" t="n">
+      <c r="C4" s="22" t="n">
         <v>100</v>
       </c>
-      <c r="D2" s="23" t="n">
+      <c r="D4" s="22" t="n">
         <v>200</v>
       </c>
-      <c r="E2" s="5" t="b">
-        <f aca="false">COUNTIF(experts!$A$2:$A$985, A2) &gt; 0</f>
-        <v>1</v>
-      </c>
-      <c r="F2" s="5" t="b">
-        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B2) &gt; 0</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="s">
+      <c r="E4" s="2" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$985, A4) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="2" t="b">
+        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$998, B4) &gt; 0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B5" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="23" t="n">
-        <v>100</v>
-      </c>
-      <c r="D3" s="23" t="n">
+      <c r="C5" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="22" t="n">
         <v>200</v>
       </c>
-      <c r="E3" s="5" t="n">
-        <f aca="false">COUNTIF(experts!$A$2:$A$985, A3) &gt; 0</f>
-        <v>1</v>
-      </c>
-      <c r="F3" s="5" t="n">
-        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B3) &gt; 0</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="s">
+      <c r="E5" s="2" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$985, A5) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F5" s="2" t="b">
+        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$998, B5) &gt; 0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B6" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="23" t="n">
-        <v>100</v>
-      </c>
-      <c r="D4" s="23" t="n">
+      <c r="C6" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="22" t="n">
         <v>200</v>
       </c>
-      <c r="E4" s="5" t="n">
-        <f aca="false">COUNTIF(experts!$A$2:$A$985, A4) &gt; 0</f>
-        <v>1</v>
-      </c>
-      <c r="F4" s="5" t="n">
-        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B4) &gt; 0</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" s="23" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="23" t="n">
-        <v>200</v>
-      </c>
-      <c r="E5" s="5" t="n">
-        <f aca="false">COUNTIF(experts!$A$2:$A$985, A5) &gt; 0</f>
-        <v>1</v>
-      </c>
-      <c r="F5" s="5" t="n">
-        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B5) &gt; 0</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" s="23" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" s="23" t="n">
-        <v>200</v>
-      </c>
-      <c r="E6" s="5" t="n">
+      <c r="E6" s="2" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$985, A6) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F6" s="5" t="n">
-        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B6) &gt; 0</f>
+      <c r="F6" s="2" t="b">
+        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$998, B6) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -1421,21 +1389,21 @@
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="23" t="s">
         <v>52</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>0</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>200</v>
-      </c>
-      <c r="E7" s="5" t="n">
+        <v>202</v>
+      </c>
+      <c r="E7" s="2" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$985, A7) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F7" s="5" t="n">
-        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B7) &gt; 0</f>
+      <c r="F7" s="2" t="b">
+        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$998, B7) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -1443,21 +1411,21 @@
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="23" t="s">
         <v>53</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>0</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>201</v>
-      </c>
-      <c r="E8" s="5" t="n">
+        <v>203</v>
+      </c>
+      <c r="E8" s="2" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$985, A8) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F8" s="5" t="n">
-        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B8) &gt; 0</f>
+      <c r="F8" s="2" t="b">
+        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$998, B8) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -1465,21 +1433,21 @@
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="23" t="s">
         <v>54</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>0</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>202</v>
-      </c>
-      <c r="E9" s="5" t="n">
+        <v>204</v>
+      </c>
+      <c r="E9" s="2" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$985, A9) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F9" s="5" t="n">
-        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B9) &gt; 0</f>
+      <c r="F9" s="2" t="b">
+        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$998, B9) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -1487,21 +1455,21 @@
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="23" t="s">
         <v>55</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>0</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>203</v>
-      </c>
-      <c r="E10" s="5" t="n">
+        <v>205</v>
+      </c>
+      <c r="E10" s="2" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$985, A10) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F10" s="5" t="n">
-        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B10) &gt; 0</f>
+      <c r="F10" s="2" t="b">
+        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$998, B10) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -1509,65 +1477,21 @@
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="23" t="s">
         <v>56</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>0</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>204</v>
-      </c>
-      <c r="E11" s="5" t="n">
+        <v>206</v>
+      </c>
+      <c r="E11" s="2" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$985, A11) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F11" s="5" t="n">
-        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B11) &gt; 0</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1" t="n">
-        <v>205</v>
-      </c>
-      <c r="E12" s="5" t="n">
-        <f aca="false">COUNTIF(experts!$A$2:$A$985, A12) &gt; 0</f>
-        <v>1</v>
-      </c>
-      <c r="F12" s="5" t="n">
-        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B12) &gt; 0</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" s="1" t="n">
-        <v>206</v>
-      </c>
-      <c r="E13" s="5" t="n">
-        <f aca="false">COUNTIF(experts!$A$2:$A$985, A13) &gt; 0</f>
-        <v>1</v>
-      </c>
-      <c r="F13" s="5" t="n">
-        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B13) &gt; 0</f>
+      <c r="F11" s="2" t="b">
+        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$998, B11) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -1596,24 +1520,24 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="11.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" s="10" t="b">
+      <c r="A1" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="9" t="b">
         <f aca="false">AND(B2:B904)</f>
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="17" t="n">
+      <c r="A2" s="16" t="n">
         <v>45651</v>
       </c>
-      <c r="B2" s="5" t="b">
+      <c r="B2" s="2" t="b">
         <f aca="false">AND(ISNUMBER(A2),misc!$A$2&lt;=A2)</f>
         <v>1</v>
       </c>
@@ -1643,94 +1567,94 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="19.48"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="3" style="25" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="19.48"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="3" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="I1" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="J1" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="K1" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="L1" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="M1" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="M1" s="26" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="17" t="n">
+      <c r="A2" s="16" t="n">
         <v>45641</v>
       </c>
-      <c r="B2" s="6" t="n">
+      <c r="B2" s="5" t="n">
         <v>8</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="D2" s="15" t="n">
+      <c r="D2" s="14" t="n">
         <v>45642</v>
       </c>
-      <c r="E2" s="15" t="n">
+      <c r="E2" s="14" t="n">
         <v>45778</v>
       </c>
-      <c r="F2" s="15" t="n">
+      <c r="F2" s="14" t="n">
         <v>45642</v>
       </c>
-      <c r="G2" s="15" t="n">
+      <c r="G2" s="14" t="n">
         <v>45778</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I2" s="27" t="n">
-        <f aca="false">MAX(MAX('invoicing periods'!C2:C900),MAX(tasks!C2:C896))</f>
+        <v>72</v>
+      </c>
+      <c r="I2" s="25" t="n">
+        <f aca="false">MAX(MAX('invoicing periods'!C2:C898),MAX(tasks!C2:C896))</f>
         <v>45795</v>
       </c>
-      <c r="J2" s="28" t="n">
+      <c r="J2" s="26" t="n">
         <f aca="false">AND(ISNUMBER(D2), D2&gt;A2)</f>
         <v>1</v>
       </c>
-      <c r="K2" s="29" t="b">
+      <c r="K2" s="27" t="b">
         <f aca="false">AND(ISNUMBER(E2), E2&lt;=I2)</f>
         <v>1</v>
       </c>
-      <c r="L2" s="29" t="b">
+      <c r="L2" s="27" t="b">
         <f aca="false">AND(ISNUMBER(F2), F2&gt;A2)</f>
         <v>1</v>
       </c>
-      <c r="M2" s="29" t="b">
+      <c r="M2" s="27" t="b">
         <f aca="false">AND(ISNUMBER(G2), G2&lt;=I2)</f>
         <v>1</v>
       </c>
@@ -1760,578 +1684,578 @@
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="6" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="5" width="11.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="5" style="2" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="10" t="b">
+      <c r="E1" s="9" t="b">
         <f aca="false">AND(E2:E899)</f>
         <v>1</v>
       </c>
-      <c r="F1" s="10" t="b">
+      <c r="F1" s="9" t="b">
         <f aca="false">AND(F2:F904)</f>
         <v>1</v>
       </c>
-      <c r="G1" s="10" t="b">
+      <c r="G1" s="9" t="b">
         <f aca="false">AND(G2:G904)</f>
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="12" t="n">
+      <c r="B2" s="11" t="n">
         <v>45642</v>
       </c>
-      <c r="C2" s="12" t="n">
+      <c r="C2" s="11" t="n">
         <v>45749</v>
       </c>
-      <c r="D2" s="13" t="n">
+      <c r="D2" s="12" t="n">
         <v>400</v>
       </c>
-      <c r="E2" s="5" t="b">
+      <c r="E2" s="2" t="b">
         <f aca="false">COUNTIF(links!$B$1:$B$868, A2) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F2" s="5" t="b">
+      <c r="F2" s="2" t="b">
         <f aca="false">C2&gt;misc!$A$2</f>
         <v>1</v>
       </c>
-      <c r="G2" s="5" t="b">
+      <c r="G2" s="2" t="b">
         <f aca="false">AND(ISNUMBER(B2), ISNUMBER(C2), B2&lt;=C2)</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="12" t="n">
+      <c r="B3" s="11" t="n">
         <v>45642</v>
       </c>
-      <c r="C3" s="12" t="n">
+      <c r="C3" s="11" t="n">
         <v>45749</v>
       </c>
-      <c r="D3" s="13" t="n">
+      <c r="D3" s="12" t="n">
         <v>420</v>
       </c>
-      <c r="E3" s="5" t="n">
+      <c r="E3" s="2" t="n">
         <f aca="false">COUNTIF(links!$B$1:$B$868, A3) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F3" s="5" t="n">
+      <c r="F3" s="2" t="n">
         <f aca="false">C3&gt;misc!$A$2</f>
         <v>1</v>
       </c>
-      <c r="G3" s="5" t="n">
+      <c r="G3" s="2" t="n">
         <f aca="false">AND(ISNUMBER(B3), ISNUMBER(C3), B3&lt;=C3)</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="12" t="n">
+      <c r="B4" s="11" t="n">
         <v>45642</v>
       </c>
-      <c r="C4" s="12" t="n">
+      <c r="C4" s="11" t="n">
         <v>45749</v>
       </c>
-      <c r="D4" s="13" t="n">
+      <c r="D4" s="12" t="n">
         <v>430</v>
       </c>
-      <c r="E4" s="5" t="n">
+      <c r="E4" s="2" t="n">
         <f aca="false">COUNTIF(links!$B$1:$B$868, A4) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F4" s="5" t="n">
+      <c r="F4" s="2" t="n">
         <f aca="false">C4&gt;misc!$A$2</f>
         <v>1</v>
       </c>
-      <c r="G4" s="5" t="n">
+      <c r="G4" s="2" t="n">
         <f aca="false">AND(ISNUMBER(B4), ISNUMBER(C4), B4&lt;=C4)</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="12" t="n">
+      <c r="B5" s="11" t="n">
         <v>45642</v>
       </c>
-      <c r="C5" s="12" t="n">
+      <c r="C5" s="11" t="n">
         <v>45749</v>
       </c>
-      <c r="D5" s="13" t="n">
+      <c r="D5" s="12" t="n">
         <v>440</v>
       </c>
-      <c r="E5" s="5" t="n">
+      <c r="E5" s="2" t="n">
         <f aca="false">COUNTIF(links!$B$1:$B$868, A5) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F5" s="5" t="n">
+      <c r="F5" s="2" t="n">
         <f aca="false">C5&gt;misc!$A$2</f>
         <v>1</v>
       </c>
-      <c r="G5" s="5" t="n">
+      <c r="G5" s="2" t="n">
         <f aca="false">AND(ISNUMBER(B5), ISNUMBER(C5), B5&lt;=C5)</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="12" t="n">
+      <c r="B6" s="11" t="n">
         <v>45642</v>
       </c>
-      <c r="C6" s="12" t="n">
+      <c r="C6" s="11" t="n">
         <v>45718</v>
       </c>
-      <c r="D6" s="13" t="n">
+      <c r="D6" s="12" t="n">
         <v>200</v>
       </c>
-      <c r="E6" s="5" t="n">
+      <c r="E6" s="2" t="n">
         <f aca="false">COUNTIF(links!$B$1:$B$868, A6) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F6" s="5" t="n">
+      <c r="F6" s="2" t="n">
         <f aca="false">C6&gt;misc!$A$2</f>
         <v>1</v>
       </c>
-      <c r="G6" s="5" t="n">
+      <c r="G6" s="2" t="n">
         <f aca="false">AND(ISNUMBER(B6), ISNUMBER(C6), B6&lt;=C6)</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="12" t="n">
+      <c r="B7" s="11" t="n">
         <v>45642</v>
       </c>
-      <c r="C7" s="12" t="n">
+      <c r="C7" s="11" t="n">
         <v>45749</v>
       </c>
-      <c r="D7" s="13" t="n">
+      <c r="D7" s="12" t="n">
         <v>200</v>
       </c>
-      <c r="E7" s="5" t="n">
+      <c r="E7" s="2" t="n">
         <f aca="false">COUNTIF(links!$B$1:$B$868, A7) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F7" s="5" t="n">
+      <c r="F7" s="2" t="n">
         <f aca="false">C7&gt;misc!$A$2</f>
         <v>1</v>
       </c>
-      <c r="G7" s="5" t="n">
+      <c r="G7" s="2" t="n">
         <f aca="false">AND(ISNUMBER(B7), ISNUMBER(C7), B7&lt;=C7)</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="12" t="n">
+      <c r="B8" s="11" t="n">
         <v>45642</v>
       </c>
-      <c r="C8" s="12" t="n">
+      <c r="C8" s="11" t="n">
         <v>45718</v>
       </c>
-      <c r="D8" s="13" t="n">
+      <c r="D8" s="12" t="n">
         <v>200</v>
       </c>
-      <c r="E8" s="5" t="n">
+      <c r="E8" s="2" t="n">
         <f aca="false">COUNTIF(links!$B$1:$B$868, A8) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F8" s="5" t="n">
+      <c r="F8" s="2" t="n">
         <f aca="false">C8&gt;misc!$A$2</f>
         <v>1</v>
       </c>
-      <c r="G8" s="5" t="n">
+      <c r="G8" s="2" t="n">
         <f aca="false">AND(ISNUMBER(B8), ISNUMBER(C8), B8&lt;=C8)</f>
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="12" t="n">
+      <c r="B9" s="11" t="n">
         <v>45642</v>
       </c>
-      <c r="C9" s="12" t="n">
+      <c r="C9" s="11" t="n">
         <v>45749</v>
       </c>
-      <c r="D9" s="13" t="n">
+      <c r="D9" s="12" t="n">
         <v>200</v>
       </c>
-      <c r="E9" s="5" t="n">
+      <c r="E9" s="2" t="n">
         <f aca="false">COUNTIF(links!$B$1:$B$868, A9) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F9" s="5" t="n">
+      <c r="F9" s="2" t="n">
         <f aca="false">C9&gt;misc!$A$2</f>
         <v>1</v>
       </c>
-      <c r="G9" s="5" t="n">
+      <c r="G9" s="2" t="n">
         <f aca="false">AND(ISNUMBER(B9), ISNUMBER(C9), B9&lt;=C9)</f>
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="12" t="n">
+      <c r="B10" s="11" t="n">
         <v>45642</v>
       </c>
-      <c r="C10" s="12" t="n">
+      <c r="C10" s="11" t="n">
         <v>45718</v>
       </c>
-      <c r="D10" s="13" t="n">
+      <c r="D10" s="12" t="n">
         <v>200</v>
       </c>
-      <c r="E10" s="5" t="n">
+      <c r="E10" s="2" t="n">
         <f aca="false">COUNTIF(links!$B$1:$B$868, A10) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F10" s="5" t="n">
+      <c r="F10" s="2" t="n">
         <f aca="false">C10&gt;misc!$A$2</f>
         <v>1</v>
       </c>
-      <c r="G10" s="5" t="n">
+      <c r="G10" s="2" t="n">
         <f aca="false">AND(ISNUMBER(B10), ISNUMBER(C10), B10&lt;=C10)</f>
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="12" t="n">
+      <c r="B11" s="11" t="n">
         <v>45642</v>
       </c>
-      <c r="C11" s="12" t="n">
+      <c r="C11" s="11" t="n">
         <v>45749</v>
       </c>
-      <c r="D11" s="13" t="n">
+      <c r="D11" s="12" t="n">
         <v>200</v>
       </c>
-      <c r="E11" s="5" t="n">
+      <c r="E11" s="2" t="n">
         <f aca="false">COUNTIF(links!$B$1:$B$868, A11) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F11" s="5" t="n">
+      <c r="F11" s="2" t="n">
         <f aca="false">C11&gt;misc!$A$2</f>
         <v>1</v>
       </c>
-      <c r="G11" s="5" t="n">
+      <c r="G11" s="2" t="n">
         <f aca="false">AND(ISNUMBER(B11), ISNUMBER(C11), B11&lt;=C11)</f>
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="12" t="n">
+      <c r="B12" s="11" t="n">
         <v>45642</v>
       </c>
-      <c r="C12" s="12" t="n">
+      <c r="C12" s="11" t="n">
         <v>45718</v>
       </c>
-      <c r="D12" s="13" t="n">
+      <c r="D12" s="12" t="n">
         <v>200</v>
       </c>
-      <c r="E12" s="5" t="n">
+      <c r="E12" s="2" t="n">
         <f aca="false">COUNTIF(links!$B$1:$B$868, A12) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F12" s="5" t="n">
+      <c r="F12" s="2" t="n">
         <f aca="false">C12&gt;misc!$A$2</f>
         <v>1</v>
       </c>
-      <c r="G12" s="5" t="n">
+      <c r="G12" s="2" t="n">
         <f aca="false">AND(ISNUMBER(B12), ISNUMBER(C12), B12&lt;=C12)</f>
         <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="12" t="n">
+      <c r="B13" s="11" t="n">
         <v>45642</v>
       </c>
-      <c r="C13" s="12" t="n">
+      <c r="C13" s="11" t="n">
         <v>45749</v>
       </c>
-      <c r="D13" s="13" t="n">
+      <c r="D13" s="12" t="n">
         <v>200</v>
       </c>
-      <c r="E13" s="5" t="n">
+      <c r="E13" s="2" t="n">
         <f aca="false">COUNTIF(links!$B$1:$B$868, A13) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F13" s="5" t="n">
+      <c r="F13" s="2" t="n">
         <f aca="false">C13&gt;misc!$A$2</f>
         <v>1</v>
       </c>
-      <c r="G13" s="5" t="n">
+      <c r="G13" s="2" t="n">
         <f aca="false">AND(ISNUMBER(B13), ISNUMBER(C13), B13&lt;=C13)</f>
         <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="12" t="n">
+      <c r="B14" s="11" t="n">
         <v>45642</v>
       </c>
-      <c r="C14" s="12" t="n">
+      <c r="C14" s="11" t="n">
         <v>45718</v>
       </c>
-      <c r="D14" s="13" t="n">
+      <c r="D14" s="12" t="n">
         <v>200</v>
       </c>
-      <c r="E14" s="5" t="n">
+      <c r="E14" s="2" t="n">
         <f aca="false">COUNTIF(links!$B$1:$B$868, A14) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F14" s="5" t="n">
+      <c r="F14" s="2" t="n">
         <f aca="false">C14&gt;misc!$A$2</f>
         <v>1</v>
       </c>
-      <c r="G14" s="5" t="n">
+      <c r="G14" s="2" t="n">
         <f aca="false">AND(ISNUMBER(B14), ISNUMBER(C14), B14&lt;=C14)</f>
         <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="12" t="n">
+      <c r="B15" s="11" t="n">
         <v>45642</v>
       </c>
-      <c r="C15" s="12" t="n">
+      <c r="C15" s="11" t="n">
         <v>45749</v>
       </c>
-      <c r="D15" s="13" t="n">
+      <c r="D15" s="12" t="n">
         <v>200</v>
       </c>
-      <c r="E15" s="5" t="n">
+      <c r="E15" s="2" t="n">
         <f aca="false">COUNTIF(links!$B$1:$B$868, A15) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F15" s="5" t="n">
+      <c r="F15" s="2" t="n">
         <f aca="false">C15&gt;misc!$A$2</f>
         <v>1</v>
       </c>
-      <c r="G15" s="5" t="n">
+      <c r="G15" s="2" t="n">
         <f aca="false">AND(ISNUMBER(B15), ISNUMBER(C15), B15&lt;=C15)</f>
         <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="12" t="n">
+      <c r="B16" s="11" t="n">
         <v>45642</v>
       </c>
-      <c r="C16" s="12" t="n">
+      <c r="C16" s="11" t="n">
         <v>45779</v>
       </c>
-      <c r="D16" s="13" t="n">
+      <c r="D16" s="12" t="n">
         <v>200</v>
       </c>
-      <c r="E16" s="5" t="n">
+      <c r="E16" s="2" t="n">
         <f aca="false">COUNTIF(links!$B$1:$B$868, A16) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F16" s="5" t="n">
+      <c r="F16" s="2" t="n">
         <f aca="false">C16&gt;misc!$A$2</f>
         <v>1</v>
       </c>
-      <c r="G16" s="5" t="n">
+      <c r="G16" s="2" t="n">
         <f aca="false">AND(ISNUMBER(B16), ISNUMBER(C16), B16&lt;=C16)</f>
         <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="12" t="n">
+      <c r="B17" s="11" t="n">
         <v>45642</v>
       </c>
-      <c r="C17" s="12" t="n">
+      <c r="C17" s="11" t="n">
         <v>45718</v>
       </c>
-      <c r="D17" s="13" t="n">
+      <c r="D17" s="12" t="n">
         <v>200</v>
       </c>
-      <c r="E17" s="5" t="n">
+      <c r="E17" s="2" t="n">
         <f aca="false">COUNTIF(links!$B$1:$B$868, A17) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F17" s="5" t="n">
+      <c r="F17" s="2" t="n">
         <f aca="false">C17&gt;misc!$A$2</f>
         <v>1</v>
       </c>
-      <c r="G17" s="5" t="n">
+      <c r="G17" s="2" t="n">
         <f aca="false">AND(ISNUMBER(B17), ISNUMBER(C17), B17&lt;=C17)</f>
         <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="12" t="n">
+      <c r="B18" s="11" t="n">
         <v>45642</v>
       </c>
-      <c r="C18" s="12" t="n">
+      <c r="C18" s="11" t="n">
         <v>45749</v>
       </c>
-      <c r="D18" s="13" t="n">
+      <c r="D18" s="12" t="n">
         <v>200</v>
       </c>
-      <c r="E18" s="5" t="n">
+      <c r="E18" s="2" t="n">
         <f aca="false">COUNTIF(links!$B$1:$B$868, A18) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F18" s="5" t="n">
+      <c r="F18" s="2" t="n">
         <f aca="false">C18&gt;misc!$A$2</f>
         <v>1</v>
       </c>
-      <c r="G18" s="5" t="n">
+      <c r="G18" s="2" t="n">
         <f aca="false">AND(ISNUMBER(B18), ISNUMBER(C18), B18&lt;=C18)</f>
         <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="12" t="n">
+      <c r="B19" s="11" t="n">
         <v>45642</v>
       </c>
-      <c r="C19" s="12" t="n">
+      <c r="C19" s="11" t="n">
         <v>45779</v>
       </c>
-      <c r="D19" s="13" t="n">
+      <c r="D19" s="12" t="n">
         <v>200</v>
       </c>
-      <c r="E19" s="5" t="n">
+      <c r="E19" s="2" t="n">
         <f aca="false">COUNTIF(links!$B$1:$B$868, A19) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F19" s="5" t="n">
+      <c r="F19" s="2" t="n">
         <f aca="false">C19&gt;misc!$A$2</f>
         <v>1</v>
       </c>
-      <c r="G19" s="5" t="n">
+      <c r="G19" s="2" t="n">
         <f aca="false">AND(ISNUMBER(B19), ISNUMBER(C19), B19&lt;=C19)</f>
         <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="12" t="n">
+      <c r="B20" s="11" t="n">
         <v>45642</v>
       </c>
-      <c r="C20" s="12" t="n">
+      <c r="C20" s="11" t="n">
         <v>45718</v>
       </c>
-      <c r="D20" s="13" t="n">
+      <c r="D20" s="12" t="n">
         <v>200</v>
       </c>
-      <c r="E20" s="5" t="n">
+      <c r="E20" s="2" t="n">
         <f aca="false">COUNTIF(links!$B$1:$B$868, A20) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F20" s="5" t="n">
+      <c r="F20" s="2" t="n">
         <f aca="false">C20&gt;misc!$A$2</f>
         <v>1</v>
       </c>
-      <c r="G20" s="5" t="n">
+      <c r="G20" s="2" t="n">
         <f aca="false">AND(ISNUMBER(B20), ISNUMBER(C20), B20&lt;=C20)</f>
         <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="12" t="n">
+      <c r="B21" s="11" t="n">
         <v>45642</v>
       </c>
-      <c r="C21" s="12" t="n">
+      <c r="C21" s="11" t="n">
         <v>45749</v>
       </c>
-      <c r="D21" s="13" t="n">
+      <c r="D21" s="12" t="n">
         <v>200</v>
       </c>
-      <c r="E21" s="5" t="n">
+      <c r="E21" s="2" t="n">
         <f aca="false">COUNTIF(links!$B$1:$B$868, A21) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F21" s="5" t="n">
+      <c r="F21" s="2" t="n">
         <f aca="false">C21&gt;misc!$A$2</f>
         <v>1</v>
       </c>
-      <c r="G21" s="5" t="n">
+      <c r="G21" s="2" t="n">
         <f aca="false">AND(ISNUMBER(B21), ISNUMBER(C21), B21&lt;=C21)</f>
         <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="12" t="n">
+      <c r="B22" s="11" t="n">
         <v>45642</v>
       </c>
-      <c r="C22" s="12" t="n">
+      <c r="C22" s="11" t="n">
         <v>45779</v>
       </c>
-      <c r="D22" s="13" t="n">
+      <c r="D22" s="12" t="n">
         <v>200</v>
       </c>
-      <c r="E22" s="5" t="n">
+      <c r="E22" s="2" t="n">
         <f aca="false">COUNTIF(links!$B$1:$B$868, A22) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F22" s="5" t="n">
+      <c r="F22" s="2" t="n">
         <f aca="false">C22&gt;misc!$A$2</f>
         <v>1</v>
       </c>
-      <c r="G22" s="5" t="n">
+      <c r="G22" s="2" t="n">
         <f aca="false">AND(ISNUMBER(B22), ISNUMBER(C22), B22&lt;=C22)</f>
         <v>1</v>
       </c>
@@ -2370,7 +2294,7 @@
       <c r="A1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>49</v>
       </c>
       <c r="C1" s="4" t="b">
@@ -2389,11 +2313,11 @@
       <c r="B2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="14" t="b">
+      <c r="C2" s="13" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$986, A2) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D2" s="14" t="b">
+      <c r="D2" s="13" t="b">
         <f aca="false">COUNTIF(tasks!$A$2:$A$903, B2) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2405,11 +2329,11 @@
       <c r="B3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="14" t="n">
+      <c r="C3" s="13" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$986, A3) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D3" s="14" t="n">
+      <c r="D3" s="13" t="n">
         <f aca="false">COUNTIF(tasks!$A$2:$A$903, B3) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2421,11 +2345,11 @@
       <c r="B4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="14" t="n">
+      <c r="C4" s="13" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$986, A4) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D4" s="14" t="n">
+      <c r="D4" s="13" t="n">
         <f aca="false">COUNTIF(tasks!$A$2:$A$903, B4) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2437,11 +2361,11 @@
       <c r="B5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="14" t="n">
+      <c r="C5" s="13" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$986, A5) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D5" s="14" t="n">
+      <c r="D5" s="13" t="n">
         <f aca="false">COUNTIF(tasks!$A$2:$A$903, B5) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2453,11 +2377,11 @@
       <c r="B6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="14" t="n">
+      <c r="C6" s="13" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$986, A6) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D6" s="14" t="n">
+      <c r="D6" s="13" t="n">
         <f aca="false">COUNTIF(tasks!$A$2:$A$903, B6) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2469,11 +2393,11 @@
       <c r="B7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="14" t="n">
+      <c r="C7" s="13" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$986, A7) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D7" s="14" t="n">
+      <c r="D7" s="13" t="n">
         <f aca="false">COUNTIF(tasks!$A$2:$A$903, B7) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2485,11 +2409,11 @@
       <c r="B8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="14" t="n">
+      <c r="C8" s="13" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$986, A8) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D8" s="14" t="n">
+      <c r="D8" s="13" t="n">
         <f aca="false">COUNTIF(tasks!$A$2:$A$903, B8) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2501,11 +2425,11 @@
       <c r="B9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="14" t="n">
+      <c r="C9" s="13" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$986, A9) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D9" s="14" t="n">
+      <c r="D9" s="13" t="n">
         <f aca="false">COUNTIF(tasks!$A$2:$A$903, B9) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2517,11 +2441,11 @@
       <c r="B10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="14" t="n">
+      <c r="C10" s="13" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$986, A10) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D10" s="14" t="n">
+      <c r="D10" s="13" t="n">
         <f aca="false">COUNTIF(tasks!$A$2:$A$903, B10) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2533,11 +2457,11 @@
       <c r="B11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="14" t="n">
+      <c r="C11" s="13" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$986, A11) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D11" s="14" t="n">
+      <c r="D11" s="13" t="n">
         <f aca="false">COUNTIF(tasks!$A$2:$A$903, B11) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2549,11 +2473,11 @@
       <c r="B12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="14" t="n">
+      <c r="C12" s="13" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$986, A12) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D12" s="14" t="n">
+      <c r="D12" s="13" t="n">
         <f aca="false">COUNTIF(tasks!$A$2:$A$903, B12) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2565,11 +2489,11 @@
       <c r="B13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="14" t="n">
+      <c r="C13" s="13" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$986, A13) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D13" s="14" t="n">
+      <c r="D13" s="13" t="n">
         <f aca="false">COUNTIF(tasks!$A$2:$A$903, B13) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2581,11 +2505,11 @@
       <c r="B14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="14" t="n">
+      <c r="C14" s="13" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$986, A14) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D14" s="14" t="n">
+      <c r="D14" s="13" t="n">
         <f aca="false">COUNTIF(tasks!$A$2:$A$903, B14) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2597,11 +2521,11 @@
       <c r="B15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="14" t="n">
+      <c r="C15" s="13" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$986, A15) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D15" s="14" t="n">
+      <c r="D15" s="13" t="n">
         <f aca="false">COUNTIF(tasks!$A$2:$A$903, B15) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2613,11 +2537,11 @@
       <c r="B16" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="14" t="n">
+      <c r="C16" s="13" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$986, A16) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D16" s="14" t="n">
+      <c r="D16" s="13" t="n">
         <f aca="false">COUNTIF(tasks!$A$2:$A$903, B16) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2629,11 +2553,11 @@
       <c r="B17" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="14" t="n">
+      <c r="C17" s="13" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$986, A17) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D17" s="14" t="n">
+      <c r="D17" s="13" t="n">
         <f aca="false">COUNTIF(tasks!$A$2:$A$903, B17) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2645,11 +2569,11 @@
       <c r="B18" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="14" t="n">
+      <c r="C18" s="13" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$986, A18) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D18" s="14" t="n">
+      <c r="D18" s="13" t="n">
         <f aca="false">COUNTIF(tasks!$A$2:$A$903, B18) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2661,11 +2585,11 @@
       <c r="B19" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="14" t="n">
+      <c r="C19" s="13" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$986, A19) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D19" s="14" t="n">
+      <c r="D19" s="13" t="n">
         <f aca="false">COUNTIF(tasks!$A$2:$A$903, B19) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2677,11 +2601,11 @@
       <c r="B20" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="14" t="n">
+      <c r="C20" s="13" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$986, A20) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D20" s="14" t="n">
+      <c r="D20" s="13" t="n">
         <f aca="false">COUNTIF(tasks!$A$2:$A$903, B20) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2693,11 +2617,11 @@
       <c r="B21" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="14" t="n">
+      <c r="C21" s="13" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$986, A21) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D21" s="14" t="n">
+      <c r="D21" s="13" t="n">
         <f aca="false">COUNTIF(tasks!$A$2:$A$903, B21) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2709,11 +2633,11 @@
       <c r="B22" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="14" t="n">
+      <c r="C22" s="13" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$986, A22) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D22" s="14" t="n">
+      <c r="D22" s="13" t="n">
         <f aca="false">COUNTIF(tasks!$A$2:$A$903, B22) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2745,7 +2669,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.76"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="3" style="6" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="3" style="5" width="11.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="7" style="2" width="11.53"/>
   </cols>
   <sheetData>
@@ -2753,19 +2677,19 @@
       <c r="A1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>51</v>
       </c>
       <c r="G1" s="4" t="b">
@@ -2776,7 +2700,7 @@
         <f aca="false">AND(H2:H934)</f>
         <v>1</v>
       </c>
-      <c r="I1" s="10" t="b">
+      <c r="I1" s="9" t="b">
         <f aca="false">AND(I2:I904)</f>
         <v>1</v>
       </c>
@@ -2788,10 +2712,10 @@
       <c r="B2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="15" t="n">
+      <c r="C2" s="14" t="n">
         <v>45642</v>
       </c>
-      <c r="D2" s="15" t="n">
+      <c r="D2" s="14" t="n">
         <v>45653</v>
       </c>
       <c r="E2" s="1" t="n">
@@ -2800,79 +2724,79 @@
       <c r="F2" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="G2" s="14" t="b">
+      <c r="G2" s="13" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$986, A2) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="H2" s="14" t="b">
+      <c r="H2" s="13" t="b">
         <f aca="false">COUNTIF(tasks!$A$2:$A$903,B2)&gt;0</f>
         <v>1</v>
       </c>
-      <c r="I2" s="5" t="b">
+      <c r="I2" s="2" t="b">
         <f aca="false">AND(ISNUMBER(C2), ISNUMBER(D2), C2&lt;=D2)</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="16" t="n">
+      <c r="C3" s="15" t="n">
         <v>45642</v>
       </c>
-      <c r="D3" s="16" t="n">
+      <c r="D3" s="15" t="n">
         <v>45646</v>
       </c>
-      <c r="E3" s="11" t="n">
+      <c r="E3" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="F3" s="11" t="n">
+      <c r="F3" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="G3" s="14" t="n">
+      <c r="G3" s="13" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$986, A3) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="H3" s="14" t="n">
+      <c r="H3" s="13" t="n">
         <f aca="false">COUNTIF(tasks!$A$2:$A$903,B3)&gt;0</f>
         <v>1</v>
       </c>
-      <c r="I3" s="5" t="n">
+      <c r="I3" s="2" t="n">
         <f aca="false">AND(ISNUMBER(C3), ISNUMBER(D3), C3&lt;=D3)</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="16" t="n">
+      <c r="C4" s="15" t="n">
         <v>45649</v>
       </c>
-      <c r="D4" s="16" t="n">
+      <c r="D4" s="15" t="n">
         <v>45653</v>
       </c>
-      <c r="E4" s="11" t="n">
+      <c r="E4" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="F4" s="11" t="n">
+      <c r="F4" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="G4" s="14" t="n">
+      <c r="G4" s="13" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$986, A4) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="H4" s="14" t="n">
+      <c r="H4" s="13" t="n">
         <f aca="false">COUNTIF(tasks!$A$2:$A$903,B4)&gt;0</f>
         <v>1</v>
       </c>
-      <c r="I4" s="5" t="n">
+      <c r="I4" s="2" t="n">
         <f aca="false">AND(ISNUMBER(C4), ISNUMBER(D4), C4&lt;=D4)</f>
         <v>1</v>
       </c>
@@ -3282,7 +3206,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.76"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="6" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="5" width="11.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="7" style="2" width="11.53"/>
   </cols>
@@ -3291,19 +3215,19 @@
       <c r="A1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>51</v>
       </c>
       <c r="G1" s="4" t="b">
@@ -3314,7 +3238,7 @@
         <f aca="false">AND(H2:H938)</f>
         <v>1</v>
       </c>
-      <c r="I1" s="10" t="b">
+      <c r="I1" s="9" t="b">
         <f aca="false">AND(I2:I908)</f>
         <v>1</v>
       </c>
@@ -3326,10 +3250,10 @@
       <c r="B2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="15" t="n">
+      <c r="C2" s="14" t="n">
         <v>45642</v>
       </c>
-      <c r="D2" s="15" t="n">
+      <c r="D2" s="14" t="n">
         <v>45646</v>
       </c>
       <c r="E2" s="1" t="n">
@@ -3338,42 +3262,33 @@
       <c r="F2" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="G2" s="5" t="b">
+      <c r="G2" s="2" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A2) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="H2" s="5" t="b">
+      <c r="H2" s="2" t="b">
         <f aca="false">COUNTIF(tasks!$A$2:$A$903,B2)&gt;0</f>
         <v>1</v>
       </c>
-      <c r="I2" s="5" t="b">
+      <c r="I2" s="2" t="b">
         <f aca="false">AND(ISNUMBER(C2), ISNUMBER(D2), C2&lt;=D2)</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
       <c r="E3" s="1"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
       <c r="E4" s="1"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
       <c r="E5" s="1"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="1"/>
@@ -3726,7 +3641,7 @@
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.76"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="2" style="6" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="2" style="5" width="11.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="6" style="2" width="11.53"/>
   </cols>
   <sheetData>
@@ -3734,23 +3649,23 @@
       <c r="A1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>51</v>
       </c>
       <c r="F1" s="4" t="b">
         <f aca="false">AND(F2:F935)</f>
         <v>1</v>
       </c>
-      <c r="G1" s="10" t="b">
+      <c r="G1" s="9" t="b">
         <f aca="false">AND(G2:G905)</f>
         <v>1</v>
       </c>
@@ -3759,10 +3674,10 @@
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="15" t="n">
+      <c r="B2" s="14" t="n">
         <v>45642</v>
       </c>
-      <c r="C2" s="15" t="n">
+      <c r="C2" s="14" t="n">
         <v>45653</v>
       </c>
       <c r="D2" s="1" t="n">
@@ -3771,11 +3686,11 @@
       <c r="E2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F2" s="5" t="b">
+      <c r="F2" s="2" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$987,A2)&gt;0</f>
         <v>1</v>
       </c>
-      <c r="G2" s="5" t="b">
+      <c r="G2" s="2" t="b">
         <f aca="false">AND(ISNUMBER(B2), ISNUMBER(C2), B2&lt;=C2)</f>
         <v>1</v>
       </c>
@@ -3784,10 +3699,10 @@
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="15" t="n">
+      <c r="B3" s="14" t="n">
         <v>45642</v>
       </c>
-      <c r="C3" s="15" t="n">
+      <c r="C3" s="14" t="n">
         <v>45653</v>
       </c>
       <c r="D3" s="1" t="n">
@@ -3796,11 +3711,11 @@
       <c r="E3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="5" t="n">
+      <c r="F3" s="2" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987,A3)&gt;0</f>
         <v>1</v>
       </c>
-      <c r="G3" s="5" t="n">
+      <c r="G3" s="2" t="n">
         <f aca="false">AND(ISNUMBER(B3), ISNUMBER(C3), B3&lt;=C3)</f>
         <v>1</v>
       </c>
@@ -3809,10 +3724,10 @@
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="15" t="n">
+      <c r="B4" s="14" t="n">
         <v>45642</v>
       </c>
-      <c r="C4" s="15" t="n">
+      <c r="C4" s="14" t="n">
         <v>45653</v>
       </c>
       <c r="D4" s="1" t="n">
@@ -3821,11 +3736,11 @@
       <c r="E4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F4" s="5" t="n">
+      <c r="F4" s="2" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987,A4)&gt;0</f>
         <v>1</v>
       </c>
-      <c r="G4" s="5" t="n">
+      <c r="G4" s="2" t="n">
         <f aca="false">AND(ISNUMBER(B4), ISNUMBER(C4), B4&lt;=C4)</f>
         <v>1</v>
       </c>
@@ -3834,10 +3749,10 @@
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="15" t="n">
+      <c r="B5" s="14" t="n">
         <v>45642</v>
       </c>
-      <c r="C5" s="15" t="n">
+      <c r="C5" s="14" t="n">
         <v>45653</v>
       </c>
       <c r="D5" s="1" t="n">
@@ -3846,38 +3761,32 @@
       <c r="E5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F5" s="5" t="n">
+      <c r="F5" s="2" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987,A5)&gt;0</f>
         <v>1</v>
       </c>
-      <c r="G5" s="5" t="n">
+      <c r="G5" s="2" t="n">
         <f aca="false">AND(ISNUMBER(B5), ISNUMBER(C5), B5&lt;=C5)</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1"/>
@@ -4278,7 +4187,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.76"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="6" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="5" width="11.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="7" style="2" width="11.53"/>
   </cols>
@@ -4287,19 +4196,19 @@
       <c r="A1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>51</v>
       </c>
       <c r="G1" s="4" t="b">
@@ -4310,7 +4219,7 @@
         <f aca="false">AND(H2:H938)</f>
         <v>1</v>
       </c>
-      <c r="I1" s="10" t="b">
+      <c r="I1" s="9" t="b">
         <f aca="false">AND(I2:I908)</f>
         <v>1</v>
       </c>
@@ -4322,10 +4231,10 @@
       <c r="B2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="15" t="n">
+      <c r="C2" s="14" t="n">
         <v>45642</v>
       </c>
-      <c r="D2" s="15" t="n">
+      <c r="D2" s="14" t="n">
         <v>45646</v>
       </c>
       <c r="E2" s="1" t="n">
@@ -4334,15 +4243,15 @@
       <c r="F2" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="G2" s="5" t="b">
+      <c r="G2" s="2" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A2) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="H2" s="5" t="b">
+      <c r="H2" s="2" t="b">
         <f aca="false">COUNTIF(tasks!$A$2:$A$903,B2)&gt;0</f>
         <v>1</v>
       </c>
-      <c r="I2" s="5" t="b">
+      <c r="I2" s="2" t="b">
         <f aca="false">AND(ISNUMBER(C2), ISNUMBER(D2), C2&lt;=D2)</f>
         <v>1</v>
       </c>
@@ -4354,10 +4263,10 @@
       <c r="B3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="15" t="n">
+      <c r="C3" s="14" t="n">
         <v>45642</v>
       </c>
-      <c r="D3" s="15" t="n">
+      <c r="D3" s="14" t="n">
         <v>45646</v>
       </c>
       <c r="E3" s="1" t="n">
@@ -4366,15 +4275,15 @@
       <c r="F3" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G3" s="5" t="n">
+      <c r="G3" s="2" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A3) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="H3" s="5" t="n">
+      <c r="H3" s="2" t="n">
         <f aca="false">COUNTIF(tasks!$A$2:$A$903,B3)&gt;0</f>
         <v>1</v>
       </c>
-      <c r="I3" s="5" t="n">
+      <c r="I3" s="2" t="n">
         <f aca="false">AND(ISNUMBER(C3), ISNUMBER(D3), C3&lt;=D3)</f>
         <v>1</v>
       </c>
@@ -4386,10 +4295,10 @@
       <c r="B4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="15" t="n">
+      <c r="C4" s="14" t="n">
         <v>45642</v>
       </c>
-      <c r="D4" s="15" t="n">
+      <c r="D4" s="14" t="n">
         <v>45646</v>
       </c>
       <c r="E4" s="1" t="n">
@@ -4398,15 +4307,15 @@
       <c r="F4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G4" s="5" t="n">
+      <c r="G4" s="2" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A4) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="H4" s="5" t="n">
+      <c r="H4" s="2" t="n">
         <f aca="false">COUNTIF(tasks!$A$2:$A$903,B4)&gt;0</f>
         <v>1</v>
       </c>
-      <c r="I4" s="5" t="n">
+      <c r="I4" s="2" t="n">
         <f aca="false">AND(ISNUMBER(C4), ISNUMBER(D4), C4&lt;=D4)</f>
         <v>1</v>
       </c>
@@ -4418,10 +4327,10 @@
       <c r="B5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="15" t="n">
+      <c r="C5" s="14" t="n">
         <v>45642</v>
       </c>
-      <c r="D5" s="15" t="n">
+      <c r="D5" s="14" t="n">
         <v>45646</v>
       </c>
       <c r="E5" s="1" t="n">
@@ -4430,15 +4339,15 @@
       <c r="F5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G5" s="5" t="n">
+      <c r="G5" s="2" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A5) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="H5" s="5" t="n">
+      <c r="H5" s="2" t="n">
         <f aca="false">COUNTIF(tasks!$A$2:$A$903,B5)&gt;0</f>
         <v>1</v>
       </c>
-      <c r="I5" s="5" t="n">
+      <c r="I5" s="2" t="n">
         <f aca="false">AND(ISNUMBER(C5), ISNUMBER(D5), C5&lt;=D5)</f>
         <v>1</v>
       </c>
@@ -4450,10 +4359,10 @@
       <c r="B6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="15" t="n">
+      <c r="C6" s="14" t="n">
         <v>45642</v>
       </c>
-      <c r="D6" s="15" t="n">
+      <c r="D6" s="14" t="n">
         <v>45646</v>
       </c>
       <c r="E6" s="1" t="n">
@@ -4462,26 +4371,23 @@
       <c r="F6" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="G6" s="5" t="n">
+      <c r="G6" s="2" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A6) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="H6" s="5" t="n">
+      <c r="H6" s="2" t="n">
         <f aca="false">COUNTIF(tasks!$A$2:$A$903,B6)&gt;0</f>
         <v>1</v>
       </c>
-      <c r="I6" s="5" t="n">
+      <c r="I6" s="2" t="n">
         <f aca="false">AND(ISNUMBER(C6), ISNUMBER(D6), C6&lt;=D6)</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
       <c r="E7" s="1"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="1"/>
@@ -4817,14 +4723,14 @@
   </sheetPr>
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="2" style="6" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="2" style="5" width="11.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="6" style="2" width="11.53"/>
   </cols>
   <sheetData>
@@ -4832,23 +4738,23 @@
       <c r="A1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>51</v>
       </c>
       <c r="F1" s="4" t="b">
         <f aca="false">AND(F2:F938)</f>
         <v>1</v>
       </c>
-      <c r="G1" s="10" t="b">
+      <c r="G1" s="9" t="b">
         <f aca="false">AND(G2:G908)</f>
         <v>1</v>
       </c>
@@ -4857,23 +4763,23 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="15" t="n">
+      <c r="B2" s="14" t="n">
         <v>45642</v>
       </c>
-      <c r="C2" s="15" t="n">
+      <c r="C2" s="14" t="n">
         <v>45689</v>
       </c>
-      <c r="D2" s="6" t="n">
+      <c r="D2" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="E2" s="6" t="n">
+      <c r="E2" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="F2" s="5" t="b">
+      <c r="F2" s="2" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$985, A2) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="G2" s="5" t="b">
+      <c r="G2" s="2" t="b">
         <f aca="false">AND(ISNUMBER(B2), ISNUMBER(C2), B2&lt;=C2)</f>
         <v>1</v>
       </c>
@@ -4882,162 +4788,162 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="15" t="n">
+      <c r="B3" s="14" t="n">
         <v>45690</v>
       </c>
-      <c r="C3" s="15" t="n">
+      <c r="C3" s="14" t="n">
         <v>45717</v>
       </c>
-      <c r="D3" s="6" t="n">
+      <c r="D3" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="E3" s="6" t="n">
+      <c r="E3" s="5" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="16"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="16"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="16"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="17"/>
-      <c r="C35" s="17"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="16"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="17"/>
-      <c r="C36" s="17"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="17"/>
-      <c r="C37" s="17"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="16"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="17"/>
-      <c r="C38" s="17"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="16"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="17"/>
-      <c r="C39" s="17"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="16"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5056,142 +4962,112 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="17" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="16" width="11.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="10" t="b">
-        <f aca="false">AND(D2:D908)</f>
+      <c r="D1" s="9" t="b">
+        <f aca="false">AND(D2:D906)</f>
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="15" t="n">
-        <v>45597</v>
-      </c>
-      <c r="C2" s="15" t="n">
-        <v>45626</v>
-      </c>
-      <c r="D2" s="5" t="b">
-        <f aca="false">AND(ISNUMBER(B2), ISNUMBER(C2), B2&lt;=C2)</f>
+      <c r="B2" s="19" t="n">
+        <v>45637</v>
+      </c>
+      <c r="C2" s="19" t="n">
+        <v>45672</v>
+      </c>
+      <c r="D2" s="2" t="b">
+        <f aca="false">AND(ISNUMBER(B2), ISNUMBER(C2), B2&lt;=C2, C2 &gt; misc!A2)</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="15" t="n">
-        <v>45627</v>
-      </c>
-      <c r="C3" s="15" t="n">
-        <v>45636</v>
-      </c>
-      <c r="D3" s="5" t="n">
-        <f aca="false">AND(ISNUMBER(B3), ISNUMBER(C3), B3&lt;=C3)</f>
+      <c r="B3" s="19" t="n">
+        <v>45673</v>
+      </c>
+      <c r="C3" s="19" t="n">
+        <v>45701</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <f aca="false">AND(ISNUMBER(B3), ISNUMBER(C3), B3&lt;=C3, C3 &gt; misc!A3)</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="20" t="n">
-        <v>45637</v>
-      </c>
-      <c r="C4" s="20" t="n">
-        <v>45672</v>
-      </c>
-      <c r="D4" s="5" t="n">
-        <f aca="false">AND(ISNUMBER(B4), ISNUMBER(C4), B4&lt;=C4)</f>
+      <c r="B4" s="19" t="n">
+        <v>45702</v>
+      </c>
+      <c r="C4" s="19" t="n">
+        <v>45732</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <f aca="false">AND(ISNUMBER(B4), ISNUMBER(C4), B4&lt;=C4, C4 &gt; misc!A4)</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="20" t="n">
-        <v>45673</v>
-      </c>
-      <c r="C5" s="20" t="n">
-        <v>45701</v>
-      </c>
-      <c r="D5" s="5" t="n">
-        <f aca="false">AND(ISNUMBER(B5), ISNUMBER(C5), B5&lt;=C5)</f>
+      <c r="B5" s="19" t="n">
+        <v>45733</v>
+      </c>
+      <c r="C5" s="19" t="n">
+        <v>45761</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <f aca="false">AND(ISNUMBER(B5), ISNUMBER(C5), B5&lt;=C5, C5 &gt; misc!A5)</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="20" t="n">
-        <v>45702</v>
-      </c>
-      <c r="C6" s="20" t="n">
-        <v>45732</v>
-      </c>
-      <c r="D6" s="5" t="n">
-        <f aca="false">AND(ISNUMBER(B6), ISNUMBER(C6), B6&lt;=C6)</f>
+      <c r="B6" s="19" t="n">
+        <v>45762</v>
+      </c>
+      <c r="C6" s="19" t="n">
+        <v>45795</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <f aca="false">AND(ISNUMBER(B6), ISNUMBER(C6), B6&lt;=C6, C6 &gt; misc!A6)</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="B7" s="20" t="n">
-        <v>45733</v>
-      </c>
-      <c r="C7" s="20" t="n">
-        <v>45761</v>
-      </c>
-      <c r="D7" s="5" t="n">
-        <f aca="false">AND(ISNUMBER(B7), ISNUMBER(C7), B7&lt;=C7)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="B8" s="20" t="n">
-        <v>45762</v>
-      </c>
-      <c r="C8" s="20" t="n">
-        <v>45795</v>
-      </c>
-      <c r="D8" s="5" t="n">
-        <f aca="false">AND(ISNUMBER(B8), ISNUMBER(C8), B8&lt;=C8)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Extend check for invoicing period interval
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/08-various-bounds/08-various-bounds.xlsx
+++ b/ampl-data-input-excel/08-various-bounds/08-various-bounds.xlsx
@@ -4965,7 +4965,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5001,7 +5001,7 @@
         <v>45672</v>
       </c>
       <c r="D2" s="2" t="b">
-        <f aca="false">AND(ISNUMBER(B2), ISNUMBER(C2), B2&lt;=C2, C2 &gt; misc!A2)</f>
+        <f aca="false">AND(ISNUMBER(B2), ISNUMBER(C2), B2&lt;=C2, C2 &gt; misc!$A$2)</f>
         <v>1</v>
       </c>
     </row>
@@ -5016,7 +5016,7 @@
         <v>45701</v>
       </c>
       <c r="D3" s="2" t="n">
-        <f aca="false">AND(ISNUMBER(B3), ISNUMBER(C3), B3&lt;=C3, C3 &gt; misc!A3)</f>
+        <f aca="false">AND(ISNUMBER(B3), ISNUMBER(C3), B3&lt;=C3, C3 &gt; misc!$A$2)</f>
         <v>1</v>
       </c>
     </row>
@@ -5031,7 +5031,7 @@
         <v>45732</v>
       </c>
       <c r="D4" s="2" t="n">
-        <f aca="false">AND(ISNUMBER(B4), ISNUMBER(C4), B4&lt;=C4, C4 &gt; misc!A4)</f>
+        <f aca="false">AND(ISNUMBER(B4), ISNUMBER(C4), B4&lt;=C4, C4 &gt; misc!$A$2)</f>
         <v>1</v>
       </c>
     </row>
@@ -5046,7 +5046,7 @@
         <v>45761</v>
       </c>
       <c r="D5" s="2" t="n">
-        <f aca="false">AND(ISNUMBER(B5), ISNUMBER(C5), B5&lt;=C5, C5 &gt; misc!A5)</f>
+        <f aca="false">AND(ISNUMBER(B5), ISNUMBER(C5), B5&lt;=C5, C5 &gt; misc!$A$2)</f>
         <v>1</v>
       </c>
     </row>
@@ -5061,7 +5061,7 @@
         <v>45795</v>
       </c>
       <c r="D6" s="2" t="n">
-        <f aca="false">AND(ISNUMBER(B6), ISNUMBER(C6), B6&lt;=C6, C6 &gt; misc!A6)</f>
+        <f aca="false">AND(ISNUMBER(B6), ISNUMBER(C6), B6&lt;=C6, C6 &gt; misc!$A$2)</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add invoicing periods bounds to example 08
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/08-various-bounds/08-various-bounds.xlsx
+++ b/ampl-data-input-excel/08-various-bounds/08-various-bounds.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="15"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="experts" sheetId="1" state="visible" r:id="rId3"/>
@@ -423,7 +423,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="97">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -1162,7 +1162,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1333,10 +1333,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1377,7 +1377,7 @@
         <v>52</v>
       </c>
       <c r="C2" s="22" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2" s="22" t="n">
         <v>200</v>
@@ -1399,7 +1399,7 @@
         <v>53</v>
       </c>
       <c r="C3" s="22" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D3" s="22" t="n">
         <v>200</v>
@@ -1421,7 +1421,7 @@
         <v>54</v>
       </c>
       <c r="C4" s="22" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D4" s="22" t="n">
         <v>200</v>
@@ -1490,7 +1490,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E7" s="2" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$985, A7) &gt; 0</f>
@@ -1512,7 +1512,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E8" s="2" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$985, A8) &gt; 0</f>
@@ -1534,7 +1534,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E9" s="2" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$985, A9) &gt; 0</f>
@@ -1556,7 +1556,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="E10" s="2" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$985, A10) &gt; 0</f>
@@ -1578,7 +1578,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="E11" s="2" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$985, A11) &gt; 0</f>
@@ -1586,6 +1586,204 @@
       </c>
       <c r="F11" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$998, B11) &gt; 0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$985, A12) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$998, B12) &gt; 0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$985, A13) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$998, B13) &gt; 0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$985, A14) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$998, B14) &gt; 0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$985, A15) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$998, B15) &gt; 0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$985, A16) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F16" s="2" t="n">
+        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$998, B16) &gt; 0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="E17" s="2" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$985, A17) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F17" s="2" t="n">
+        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$998, B17) &gt; 0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="E18" s="2" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$985, A18) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F18" s="2" t="n">
+        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$998, B18) &gt; 0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="E19" s="2" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$985, A19) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F19" s="2" t="n">
+        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$998, B19) &gt; 0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="E20" s="2" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$985, A20) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F20" s="2" t="n">
+        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$998, B20) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -1996,7 +2194,7 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>

</xml_diff>